<commit_message>
some more excel files plus updated solver
solver doesn't need excel and plots in python
</commit_message>
<xml_diff>
--- a/optimize 1.xlsx
+++ b/optimize 1.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Chris\PycharmProjects\ride_solver\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mackr\OneDrive\Documents\python_projects\rider solver\ride_solver\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2B02698-7E66-441B-9D9E-B1705074F3BC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C0C2832-A2EF-4397-BF67-7EF83F0A7921}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{D30F47EA-90C8-427E-9981-7FBDEA5670DF}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="22695" windowHeight="14746" xr2:uid="{D30F47EA-90C8-427E-9981-7FBDEA5670DF}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -70,7 +70,9 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -918,100 +920,100 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="47"/>
                 <c:pt idx="0">
-                  <c:v>-0.89905322734774096</c:v>
+                  <c:v>5.3622772123000004</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3.3333333333333335</c:v>
+                  <c:v>0.80693497749999998</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.81178188793316886</c:v>
+                  <c:v>0.57338012189999998</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.57540684173199919</c:v>
+                  <c:v>0.46218115119999997</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.46330762212964116</c:v>
+                  <c:v>0.39808266819999999</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.39881017670979807</c:v>
+                  <c:v>0.35753703440000001</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>-2.8506498523888202</c:v>
+                  <c:v>-4.0937250163999996</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>-5.5973725128120009</c:v>
+                  <c:v>-5.5972379218999997</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>-5.0382954994443523</c:v>
+                  <c:v>-5.0382281794999999</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>-2.7209718999853165</c:v>
+                  <c:v>-2.7209796920999998</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>-2.2941408826284087</c:v>
+                  <c:v>-2.2941013434999999</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.68827144075275781</c:v>
+                  <c:v>0.68823917550000002</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.52065749453103116</c:v>
+                  <c:v>0.52063085279999999</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0.43278014883994498</c:v>
+                  <c:v>0.43275222940000002</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0.37987452904105873</c:v>
+                  <c:v>0.37984543650000002</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0.3456267544683212</c:v>
+                  <c:v>0.34559664559999997</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0.32248097873156589</c:v>
+                  <c:v>0.3224500045</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0.30640476169421088</c:v>
+                  <c:v>0.30637304510000002</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>0.29503511815930472</c:v>
+                  <c:v>0.29500274479999999</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>0.2868946727906857</c:v>
+                  <c:v>0.28686168490000002</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>0.28101635478366221</c:v>
+                  <c:v>0.28098274690000002</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>0.2767459772718156</c:v>
+                  <c:v>0.27671168730000001</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>0.27363040817363604</c:v>
+                  <c:v>0.27359530310000002</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>0.27135036283896757</c:v>
+                  <c:v>0.27131421259999999</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>0.26967805907043779</c:v>
+                  <c:v>0.26964048979999999</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>0.268449520522833</c:v>
+                  <c:v>0.26840992600000002</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>0.26754592386506326</c:v>
+                  <c:v>0.26750328699999998</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>0.26688074984697091</c:v>
+                  <c:v>0.26683323920000002</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>0.26639077833742736</c:v>
+                  <c:v>0.26633466859999999</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>0.26602969429639273</c:v>
+                  <c:v>0.26595558380000001</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>0.26576350275494681</c:v>
+                  <c:v>0.26563357199999998</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>0</c:v>
+                  <c:v>-1.6307550583999999</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1172,100 +1174,100 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="32"/>
                 <c:pt idx="0">
-                  <c:v>0.89905322734774096</c:v>
+                  <c:v>5.3622772123000004</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3.3333334833333299</c:v>
+                  <c:v>0.80711534692475162</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.81195696988029709</c:v>
+                  <c:v>0.57437498341003002</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.57638462148486069</c:v>
+                  <c:v>0.46509759197264378</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.46619025145351367</c:v>
+                  <c:v>0.40420574990667851</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.4048825715636763</c:v>
+                  <c:v>0.36793546728835297</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>2.8519664430269036</c:v>
+                  <c:v>4.0949854316949281</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>5.597831427165497</c:v>
+                  <c:v>5.5976968104917448</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>5.0384620262732547</c:v>
+                  <c:v>5.038394700885652</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>5.5553342961828509</c:v>
+                  <c:v>5.5552856149755314</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>5.092627952709516</c:v>
+                  <c:v>5.0925565472530172</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>4.7412506238380852</c:v>
+                  <c:v>4.7412292553742175</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.52226833695967678</c:v>
+                  <c:v>8.2139890579946861</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0.43682704934707761</c:v>
+                  <c:v>11.872376492997102</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0.38759938974323244</c:v>
+                  <c:v>15.404051629192585</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0.35792350717793392</c:v>
+                  <c:v>0.35789418246526444</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0.33971985083905859</c:v>
+                  <c:v>0.33969008853437815</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0.32846687031568633</c:v>
+                  <c:v>0.32843681848913847</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>0.32146451811393595</c:v>
+                  <c:v>0.32143424723797887</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>0.31706745368884315</c:v>
+                  <c:v>0.31703696773190487</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>0.31427169772332786</c:v>
+                  <c:v>0.31424094588202917</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>0.31246649793776793</c:v>
+                  <c:v>0.31243537761145967</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>0.31128064559250979</c:v>
+                  <c:v>29.680578852887297</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>0.31048769597079984</c:v>
+                  <c:v>0.31045527836309933</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>0.30994831480241403</c:v>
+                  <c:v>0.3099147722329898</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>0.30957563777536756</c:v>
+                  <c:v>30.837109594329618</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>0.30931460857243614</c:v>
+                  <c:v>0.30927680928719814</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>0.3091296728474473</c:v>
+                  <c:v>0.309087690788511</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>0.3089974182198939</c:v>
+                  <c:v>0.30894801652795845</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>0.30890213119263354</c:v>
+                  <c:v>0.30883717567364855</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>0.30883307786462261</c:v>
+                  <c:v>0.30871994855650986</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>0.15754643009057179</c:v>
+                  <c:v>1.6383472799478473</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1418,97 +1420,97 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1E-3</c:v>
+                  <c:v>1.7062395158262585E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.6860823255513788E-2</c:v>
+                  <c:v>3.3791380220603719E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3.3558879186470741E-2</c:v>
+                  <c:v>5.2003399256150669E-2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>5.1762900101017827E-2</c:v>
+                  <c:v>7.0089068594104409E-2</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>6.9859428202033516E-2</c:v>
+                  <c:v>8.6854919959388863E-2</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>8.6648780875016138E-2</c:v>
+                  <c:v>0.10159318822893371</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>7.167733099364193E-2</c:v>
+                  <c:v>7.1674457333267674E-2</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>4.0964014407459712E-2</c:v>
+                  <c:v>4.0963071231762287E-2</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>4.8433512222257544</c:v>
+                  <c:v>4.8432910070667301</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>4.5466226009392141</c:v>
+                  <c:v>4.5465625710773043</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>4.6910275955156298</c:v>
+                  <c:v>4.6910107321688619</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>4.098767106455084E-2</c:v>
+                  <c:v>-8.1974727666500478</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>5.9322961923265839E-2</c:v>
+                  <c:v>-11.864486887321318</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>7.6997591619218875E-2</c:v>
+                  <c:v>-15.399367650627763</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>9.3012814097022792E-2</c:v>
+                  <c:v>9.3011850817559902E-2</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0.10684378976076975</c:v>
+                  <c:v>0.10684264526135459</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0.11834951164282742</c:v>
+                  <c:v>0.11834821914765195</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>0.12764683881299271</c:v>
+                  <c:v>0.12764543022729874</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>0.13499339581272884</c:v>
+                  <c:v>0.13499189844199536</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>0.14070006515281236</c:v>
+                  <c:v>0.14069850039486179</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>0.14507576088844357</c:v>
+                  <c:v>0.14507414412913974</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>0.14839824811371266</c:v>
+                  <c:v>29.679317826604141</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>0.15090258426023226</c:v>
+                  <c:v>0.15090088768708917</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>0.15277991459893481</c:v>
+                  <c:v>0.15277818008027857</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>0.15418148538357856</c:v>
+                  <c:v>30.835941435998357</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>0.15522469423229396</c:v>
+                  <c:v>0.15522285980829489</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>0.15599942306267783</c:v>
+                  <c:v>0.1559975097718222</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>0.15657380905930487</c:v>
+                  <c:v>0.1565717765700059</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>0.15699913505468366</c:v>
+                  <c:v>0.15699690609587574</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>0.15731379655566588</c:v>
+                  <c:v>0.15731119497116197</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>0.15754643009057179</c:v>
+                  <c:v>0.15754284882317873</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1670,97 +1672,97 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1</c:v>
+                  <c:v>4.1306652198238707</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4.1061932803405377</c:v>
+                  <c:v>5.8130353706651157</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>5.7930026054258548</c:v>
+                  <c:v>7.2113382430829489</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>7.194643848101018</c:v>
+                  <c:v>8.3719214397953117</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>8.3581952718295298</c:v>
+                  <c:v>9.3195987016281379</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>9.3085326918379643</c:v>
+                  <c:v>10.07934463290812</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>8.4662465705672627</c:v>
+                  <c:v>8.4660768560926538</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>6.4003136178987132</c:v>
+                  <c:v>6.4002399354838477</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>4.9210523377758104</c:v>
+                  <c:v>4.9210217470900952</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>4.767925440345735</c:v>
+                  <c:v>4.7678939643606295</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>4.8430504826584402</c:v>
+                  <c:v>4.8430417777306349</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>6.4021614369329081</c:v>
+                  <c:v>6.4021374425460627</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>7.7021400872267858</c:v>
+                  <c:v>7.7021058442874306</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>8.7748271560879694</c:v>
+                  <c:v>8.7747842282952355</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>9.6443151180901801</c:v>
+                  <c:v>9.6442651776877177</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>10.336526968027982</c:v>
+                  <c:v>10.33647160598599</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>10.878856173459939</c:v>
+                  <c:v>10.878796769296315</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>11.29809005155264</c:v>
+                  <c:v>11.298027714043666</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>11.618665836176236</c:v>
+                  <c:v>11.61860139784455</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>11.861705828118161</c:v>
+                  <c:v>11.861639869548467</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>12.044739967655739</c:v>
+                  <c:v>12.044672852723719</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>12.181881961081082</c:v>
+                  <c:v>12.181813868756192</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>12.284241297704643</c:v>
+                  <c:v>12.284172242649856</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>12.360417250195674</c:v>
+                  <c:v>12.360347085752835</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>12.416983747415415</c:v>
+                  <c:v>12.41691214352392</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>12.458920267514916</c:v>
+                  <c:v>12.458846648397872</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>12.489972900798378</c:v>
+                  <c:v>12.489896307488793</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>12.512945658768956</c:v>
+                  <c:v>12.512864443044442</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>12.529929571018492</c:v>
+                  <c:v>12.529840625318254</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>12.542479681293722</c:v>
+                  <c:v>12.542375969933367</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>12.551750080788407</c:v>
+                  <c:v>12.551607419895618</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2831,97 +2833,97 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1E-3</c:v>
+                  <c:v>1.7062395158262585E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.6860823255513788E-2</c:v>
+                  <c:v>3.3791380220603719E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3.3558879186470741E-2</c:v>
+                  <c:v>5.2003399256150669E-2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>5.1762900101017827E-2</c:v>
+                  <c:v>7.0089068594104409E-2</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>6.9859428202033516E-2</c:v>
+                  <c:v>8.6854919959388863E-2</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>8.6648780875016138E-2</c:v>
+                  <c:v>0.10159318822893371</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>7.167733099364193E-2</c:v>
+                  <c:v>7.1674457333267674E-2</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>4.0964014407459712E-2</c:v>
+                  <c:v>4.0963071231762287E-2</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>4.8433512222257544</c:v>
+                  <c:v>4.8432910070667301</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>4.5466226009392141</c:v>
+                  <c:v>4.5465625710773043</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>4.6910275955156298</c:v>
+                  <c:v>4.6910107321688619</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>4.098767106455084E-2</c:v>
+                  <c:v>-8.1974727666500478</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>5.9322961923265839E-2</c:v>
+                  <c:v>-11.864486887321318</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>7.6997591619218875E-2</c:v>
+                  <c:v>-15.399367650627763</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>9.3012814097022792E-2</c:v>
+                  <c:v>9.3011850817559902E-2</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0.10684378976076975</c:v>
+                  <c:v>0.10684264526135459</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0.11834951164282742</c:v>
+                  <c:v>0.11834821914765195</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>0.12764683881299271</c:v>
+                  <c:v>0.12764543022729874</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>0.13499339581272884</c:v>
+                  <c:v>0.13499189844199536</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>0.14070006515281236</c:v>
+                  <c:v>0.14069850039486179</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>0.14507576088844357</c:v>
+                  <c:v>0.14507414412913974</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>0.14839824811371266</c:v>
+                  <c:v>29.679317826604141</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>0.15090258426023226</c:v>
+                  <c:v>0.15090088768708917</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>0.15277991459893481</c:v>
+                  <c:v>0.15277818008027857</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>0.15418148538357856</c:v>
+                  <c:v>30.835941435998357</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>0.15522469423229396</c:v>
+                  <c:v>0.15522285980829489</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>0.15599942306267783</c:v>
+                  <c:v>0.1559975097718222</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>0.15657380905930487</c:v>
+                  <c:v>0.1565717765700059</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>0.15699913505468366</c:v>
+                  <c:v>0.15699690609587574</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>0.15731379655566588</c:v>
+                  <c:v>0.15731119497116197</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>0.15754643009057179</c:v>
+                  <c:v>0.15754284882317873</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2933,100 +2935,100 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="32"/>
                 <c:pt idx="0">
-                  <c:v>-0.89905322734774096</c:v>
+                  <c:v>5.3622772123000004</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3.3333333333333335</c:v>
+                  <c:v>0.80693497749999998</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.81178188793316886</c:v>
+                  <c:v>0.57338012189999998</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.57540684173199919</c:v>
+                  <c:v>0.46218115119999997</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.46330762212964116</c:v>
+                  <c:v>0.39808266819999999</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.39881017670979807</c:v>
+                  <c:v>0.35753703440000001</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>-2.8506498523888202</c:v>
+                  <c:v>-4.0937250163999996</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>-5.5973725128120009</c:v>
+                  <c:v>-5.5972379218999997</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>-5.0382954994443523</c:v>
+                  <c:v>-5.0382281794999999</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>-2.7209718999853165</c:v>
+                  <c:v>-2.7209796920999998</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>-2.2941408826284087</c:v>
+                  <c:v>-2.2941013434999999</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.68827144075275781</c:v>
+                  <c:v>0.68823917550000002</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.52065749453103116</c:v>
+                  <c:v>0.52063085279999999</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0.43278014883994498</c:v>
+                  <c:v>0.43275222940000002</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0.37987452904105873</c:v>
+                  <c:v>0.37984543650000002</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0.3456267544683212</c:v>
+                  <c:v>0.34559664559999997</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0.32248097873156589</c:v>
+                  <c:v>0.3224500045</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0.30640476169421088</c:v>
+                  <c:v>0.30637304510000002</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>0.29503511815930472</c:v>
+                  <c:v>0.29500274479999999</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>0.2868946727906857</c:v>
+                  <c:v>0.28686168490000002</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>0.28101635478366221</c:v>
+                  <c:v>0.28098274690000002</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>0.2767459772718156</c:v>
+                  <c:v>0.27671168730000001</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>0.27363040817363604</c:v>
+                  <c:v>0.27359530310000002</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>0.27135036283896757</c:v>
+                  <c:v>0.27131421259999999</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>0.26967805907043779</c:v>
+                  <c:v>0.26964048979999999</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>0.268449520522833</c:v>
+                  <c:v>0.26840992600000002</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>0.26754592386506326</c:v>
+                  <c:v>0.26750328699999998</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>0.26688074984697091</c:v>
+                  <c:v>0.26683323920000002</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>0.26639077833742736</c:v>
+                  <c:v>0.26633466859999999</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>0.26602969429639273</c:v>
+                  <c:v>0.26595558380000001</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>0.26576350275494681</c:v>
+                  <c:v>0.26563357199999998</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>0</c:v>
+                  <c:v>-1.6307550583999999</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3595,13 +3597,13 @@
                   <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>1000</c:v>
+                  <c:v>-5</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>1000</c:v>
+                  <c:v>-5</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>1000</c:v>
+                  <c:v>-5</c:v>
                 </c:pt>
                 <c:pt idx="15">
                   <c:v>1000</c:v>
@@ -3625,7 +3627,7 @@
                   <c:v>1000</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>1000</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="23">
                   <c:v>1000</c:v>
@@ -3634,7 +3636,7 @@
                   <c:v>1000</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>1000</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="26">
                   <c:v>1000</c:v>
@@ -3820,100 +3822,100 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="32"/>
                 <c:pt idx="0">
-                  <c:v>0.89905322734774096</c:v>
+                  <c:v>-5.3622772123000004</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>-3.3333333333333335</c:v>
+                  <c:v>-0.80693497749999998</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>-0.81178188793316886</c:v>
+                  <c:v>-0.57338012189999998</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>-0.57540684173199919</c:v>
+                  <c:v>-0.46218115119999997</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>-0.46330762212964116</c:v>
+                  <c:v>-0.39808266819999999</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>-0.39881017670979807</c:v>
+                  <c:v>-0.35753703440000001</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>2.8506498523888202</c:v>
+                  <c:v>4.0937250163999996</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>5.5973725128120009</c:v>
+                  <c:v>5.5972379218999997</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>5.0382954994443523</c:v>
+                  <c:v>5.0382281794999999</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>2.7209718999853165</c:v>
+                  <c:v>2.7209796920999998</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>2.2941408826284087</c:v>
+                  <c:v>2.2941013434999999</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>-0.68827144075275781</c:v>
+                  <c:v>-0.68823917550000002</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>-0.52065749453103116</c:v>
+                  <c:v>-0.52063085279999999</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>-0.43278014883994498</c:v>
+                  <c:v>-0.43275222940000002</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>-0.37987452904105873</c:v>
+                  <c:v>-0.37984543650000002</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>-0.3456267544683212</c:v>
+                  <c:v>-0.34559664559999997</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>-0.32248097873156589</c:v>
+                  <c:v>-0.3224500045</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>-0.30640476169421088</c:v>
+                  <c:v>-0.30637304510000002</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>-0.29503511815930472</c:v>
+                  <c:v>-0.29500274479999999</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>-0.2868946727906857</c:v>
+                  <c:v>-0.28686168490000002</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>-0.28101635478366221</c:v>
+                  <c:v>-0.28098274690000002</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>-0.2767459772718156</c:v>
+                  <c:v>-0.27671168730000001</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>-0.27363040817363604</c:v>
+                  <c:v>-0.27359530310000002</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>-0.27135036283896757</c:v>
+                  <c:v>-0.27131421259999999</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>-0.26967805907043779</c:v>
+                  <c:v>-0.26964048979999999</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>-0.268449520522833</c:v>
+                  <c:v>-0.26840992600000002</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>-0.26754592386506326</c:v>
+                  <c:v>-0.26750328699999998</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>-0.26688074984697091</c:v>
+                  <c:v>-0.26683323920000002</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>-0.26639077833742736</c:v>
+                  <c:v>-0.26633466859999999</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>-0.26602969429639273</c:v>
+                  <c:v>-0.26595558380000001</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>-0.26576350275494681</c:v>
+                  <c:v>-0.26563357199999998</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>0</c:v>
+                  <c:v>1.6307550583999999</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4585,97 +4587,97 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1</c:v>
+                  <c:v>4.1306652198238707</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4.1061932803405377</c:v>
+                  <c:v>5.8130353706651157</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>5.7930026054258548</c:v>
+                  <c:v>7.2113382430829489</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>7.194643848101018</c:v>
+                  <c:v>8.3719214397953117</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>8.3581952718295298</c:v>
+                  <c:v>9.3195987016281379</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>9.3085326918379643</c:v>
+                  <c:v>10.07934463290812</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>8.4662465705672627</c:v>
+                  <c:v>8.4660768560926538</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>6.4003136178987132</c:v>
+                  <c:v>6.4002399354838477</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>4.9210523377758104</c:v>
+                  <c:v>4.9210217470900952</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>4.767925440345735</c:v>
+                  <c:v>4.7678939643606295</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>4.8430504826584402</c:v>
+                  <c:v>4.8430417777306349</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>6.4021614369329081</c:v>
+                  <c:v>6.4021374425460627</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>7.7021400872267858</c:v>
+                  <c:v>7.7021058442874306</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>8.7748271560879694</c:v>
+                  <c:v>8.7747842282952355</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>9.6443151180901801</c:v>
+                  <c:v>9.6442651776877177</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>10.336526968027982</c:v>
+                  <c:v>10.33647160598599</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>10.878856173459939</c:v>
+                  <c:v>10.878796769296315</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>11.29809005155264</c:v>
+                  <c:v>11.298027714043666</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>11.618665836176236</c:v>
+                  <c:v>11.61860139784455</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>11.861705828118161</c:v>
+                  <c:v>11.861639869548467</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>12.044739967655739</c:v>
+                  <c:v>12.044672852723719</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>12.181881961081082</c:v>
+                  <c:v>12.181813868756192</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>12.284241297704643</c:v>
+                  <c:v>12.284172242649856</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>12.360417250195674</c:v>
+                  <c:v>12.360347085752835</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>12.416983747415415</c:v>
+                  <c:v>12.41691214352392</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>12.458920267514916</c:v>
+                  <c:v>12.458846648397872</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>12.489972900798378</c:v>
+                  <c:v>12.489896307488793</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>12.512945658768956</c:v>
+                  <c:v>12.512864443044442</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>12.529929571018492</c:v>
+                  <c:v>12.529840625318254</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>12.542479681293722</c:v>
+                  <c:v>12.542375969933367</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>12.551750080788407</c:v>
+                  <c:v>12.551607419895618</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4867,13 +4869,13 @@
                   <c:v>4.8476798574163293</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>68.556546004010443</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>68.556546004010443</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>68.556546004010443</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="15">
                   <c:v>68.556546004010443</c:v>
@@ -4897,7 +4899,7 @@
                   <c:v>68.556546004010443</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>68.556546004010443</c:v>
+                  <c:v>4.8476798574163293</c:v>
                 </c:pt>
                 <c:pt idx="23">
                   <c:v>68.556546004010443</c:v>
@@ -4906,7 +4908,7 @@
                   <c:v>68.556546004010443</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>68.556546004010443</c:v>
+                  <c:v>4.8476798574163293</c:v>
                 </c:pt>
                 <c:pt idx="26">
                   <c:v>68.556546004010443</c:v>
@@ -7508,16 +7510,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>478757</xdr:colOff>
-      <xdr:row>23</xdr:row>
-      <xdr:rowOff>73902</xdr:rowOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>567203</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>67097</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>21</xdr:col>
+      <xdr:col>20</xdr:col>
       <xdr:colOff>112453</xdr:colOff>
-      <xdr:row>56</xdr:row>
-      <xdr:rowOff>98072</xdr:rowOff>
+      <xdr:row>65</xdr:row>
+      <xdr:rowOff>91269</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -7964,34 +7966,34 @@
   <dimension ref="A1:AE40"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="Y23" sqref="Y23"/>
+      <selection activeCell="J29" sqref="J29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="9" customWidth="1"/>
-    <col min="2" max="2" width="4.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="20.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="18.42578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="5.5703125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="12" max="13" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="14.5703125" customWidth="1"/>
-    <col min="16" max="16" width="16.7109375" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="15.7109375" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="4.86328125" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="11.86328125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.265625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.1328125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.59765625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18.3984375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.3984375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="5.59765625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.86328125" bestFit="1" customWidth="1"/>
+    <col min="12" max="13" width="14.265625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="15.265625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="14.59765625" customWidth="1"/>
+    <col min="16" max="16" width="16.73046875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="15.73046875" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="11.73046875" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="16" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="21" max="22" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="12.1328125" bestFit="1" customWidth="1"/>
+    <col min="21" max="22" width="12.3984375" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="11.86328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:31" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:31" ht="18" x14ac:dyDescent="0.55000000000000004">
       <c r="B1" t="s">
         <v>3</v>
       </c>
@@ -8020,7 +8022,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:31" x14ac:dyDescent="0.45">
       <c r="B2" t="s">
         <v>4</v>
       </c>
@@ -8047,7 +8049,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="3" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:31" x14ac:dyDescent="0.45">
       <c r="A3" s="1"/>
       <c r="B3" s="19" t="s">
         <v>0</v>
@@ -8093,7 +8095,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="4" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:31" x14ac:dyDescent="0.45">
       <c r="B4" s="7">
         <v>0</v>
       </c>
@@ -8105,11 +8107,11 @@
         <v>2.899053227347741</v>
       </c>
       <c r="E4" s="18">
-        <v>-0.89905322734774096</v>
+        <v>5.3622772123000004</v>
       </c>
       <c r="F4" s="7">
         <f>D4+E4-0.02*K4^2</f>
-        <v>2</v>
+        <v>8.2613304396477414</v>
       </c>
       <c r="G4" s="7"/>
       <c r="H4" s="7">
@@ -8131,7 +8133,7 @@
       </c>
       <c r="M4" s="7">
         <f t="shared" ref="M4:M35" si="3">SQRT((L4)^2+E4^2)</f>
-        <v>0.89905322734774096</v>
+        <v>5.3622772123000004</v>
       </c>
       <c r="N4" s="15">
         <f t="shared" ref="N4:N35" si="4">-I4</f>
@@ -8146,7 +8148,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:31" x14ac:dyDescent="0.45">
       <c r="B5" s="7">
         <f>B4+0.5</f>
         <v>0.5</v>
@@ -8159,11 +8161,11 @@
         <v>2.899053227347741</v>
       </c>
       <c r="E5" s="18">
-        <v>3.3333333333333335</v>
+        <v>0.80693497749999998</v>
       </c>
       <c r="F5" s="7">
         <f t="shared" ref="F5:F35" si="6">D5+E5-0.02*K5^2</f>
-        <v>6.2123865606810753</v>
+        <v>3.3647403016824895</v>
       </c>
       <c r="G5" s="7"/>
       <c r="H5" s="7">
@@ -8178,15 +8180,15 @@
       </c>
       <c r="K5" s="15">
         <f>F4*(B5-B4) + K4</f>
-        <v>1</v>
+        <v>4.1306652198238707</v>
       </c>
       <c r="L5" s="7">
         <f t="shared" si="2"/>
-        <v>1E-3</v>
+        <v>1.7062395158262585E-2</v>
       </c>
       <c r="M5" s="7">
         <f>SQRT((L5)^2+E5^2)</f>
-        <v>3.3333334833333299</v>
+        <v>0.80711534692475162</v>
       </c>
       <c r="N5" s="15">
         <f t="shared" si="4"/>
@@ -8194,14 +8196,14 @@
       </c>
       <c r="O5" s="13">
         <f t="shared" si="5"/>
-        <v>500</v>
+        <v>499.97673693279114</v>
       </c>
       <c r="P5" s="21">
         <f t="shared" ref="P5:P35" si="7">IF(O5&gt;0,P4+O5*(B5-B4),P4)</f>
-        <v>250</v>
+        <v>249.98836846639557</v>
       </c>
     </row>
-    <row r="6" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:31" x14ac:dyDescent="0.45">
       <c r="B6" s="7">
         <f t="shared" ref="B6:B35" si="8">B5+0.5</f>
         <v>1</v>
@@ -8214,11 +8216,11 @@
         <v>2.899053227347741</v>
       </c>
       <c r="E6" s="18">
-        <v>0.81178188793316886</v>
+        <v>0.57338012189999998</v>
       </c>
       <c r="F6" s="7">
         <f t="shared" si="6"/>
-        <v>3.3736186501706338</v>
+        <v>2.7966057448356665</v>
       </c>
       <c r="G6" s="7"/>
       <c r="H6" s="7">
@@ -8233,15 +8235,15 @@
       </c>
       <c r="K6" s="15">
         <f t="shared" ref="K6:K35" si="9">F5*(B6-B5) + K5</f>
-        <v>4.1061932803405377</v>
+        <v>5.8130353706651157</v>
       </c>
       <c r="L6" s="7">
         <f t="shared" si="2"/>
-        <v>1.6860823255513788E-2</v>
+        <v>3.3791380220603719E-2</v>
       </c>
       <c r="M6" s="7">
         <f t="shared" si="3"/>
-        <v>0.81195696988029709</v>
+        <v>0.57437498341003002</v>
       </c>
       <c r="N6" s="15">
         <f t="shared" si="4"/>
@@ -8249,14 +8251,14 @@
       </c>
       <c r="O6" s="13">
         <f t="shared" si="5"/>
-        <v>500</v>
+        <v>499.96183941614635</v>
       </c>
       <c r="P6" s="21">
         <f t="shared" si="7"/>
-        <v>500</v>
+        <v>499.96928817446872</v>
       </c>
     </row>
-    <row r="7" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:31" x14ac:dyDescent="0.45">
       <c r="B7" s="7">
         <f t="shared" si="8"/>
         <v>1.5</v>
@@ -8269,11 +8271,11 @@
         <v>2.899053227347741</v>
       </c>
       <c r="E7" s="18">
-        <v>0.57540684173199919</v>
+        <v>0.46218115119999997</v>
       </c>
       <c r="F7" s="7">
         <f t="shared" si="6"/>
-        <v>2.8032824853503255</v>
+        <v>2.3211663934247273</v>
       </c>
       <c r="G7" s="7"/>
       <c r="H7" s="7">
@@ -8288,15 +8290,15 @@
       </c>
       <c r="K7" s="15">
         <f t="shared" si="9"/>
-        <v>5.7930026054258548</v>
+        <v>7.2113382430829489</v>
       </c>
       <c r="L7" s="7">
         <f t="shared" si="2"/>
-        <v>3.3558879186470741E-2</v>
+        <v>5.2003399256150669E-2</v>
       </c>
       <c r="M7" s="7">
         <f t="shared" si="3"/>
-        <v>0.57638462148486069</v>
+        <v>0.46509759197264378</v>
       </c>
       <c r="N7" s="15">
         <f t="shared" si="4"/>
@@ -8304,14 +8306,14 @@
       </c>
       <c r="O7" s="13">
         <f t="shared" si="5"/>
-        <v>500.00000000000006</v>
+        <v>499.94169163209932</v>
       </c>
       <c r="P7" s="21">
         <f t="shared" si="7"/>
-        <v>750</v>
+        <v>749.94013399051835</v>
       </c>
     </row>
-    <row r="8" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:31" x14ac:dyDescent="0.45">
       <c r="B8" s="7">
         <f t="shared" si="8"/>
         <v>2</v>
@@ -8324,11 +8326,11 @@
         <v>2.899053227347741</v>
       </c>
       <c r="E8" s="18">
-        <v>0.46330762212964116</v>
+        <v>0.39808266819999999</v>
       </c>
       <c r="F8" s="7">
         <f t="shared" si="6"/>
-        <v>2.3271028474570254</v>
+        <v>1.8953545236656526</v>
       </c>
       <c r="G8" s="7"/>
       <c r="H8" s="7">
@@ -8343,15 +8345,15 @@
       </c>
       <c r="K8" s="15">
         <f t="shared" si="9"/>
-        <v>7.194643848101018</v>
+        <v>8.3719214397953117</v>
       </c>
       <c r="L8" s="7">
         <f t="shared" si="2"/>
-        <v>5.1762900101017827E-2</v>
+        <v>7.0089068594104409E-2</v>
       </c>
       <c r="M8" s="7">
         <f t="shared" si="3"/>
-        <v>0.46619025145351367</v>
+        <v>0.40420574990667851</v>
       </c>
       <c r="N8" s="15">
         <f t="shared" si="4"/>
@@ -8359,14 +8361,14 @@
       </c>
       <c r="O8" s="13">
         <f t="shared" si="5"/>
-        <v>500.00000000000011</v>
+        <v>499.90752370717553</v>
       </c>
       <c r="P8" s="21">
         <f t="shared" si="7"/>
-        <v>1000</v>
+        <v>999.89389584410605</v>
       </c>
     </row>
-    <row r="9" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:31" x14ac:dyDescent="0.45">
       <c r="B9" s="7">
         <f t="shared" si="8"/>
         <v>2.5</v>
@@ -8379,11 +8381,11 @@
         <v>2.899053227347741</v>
       </c>
       <c r="E9" s="18">
-        <v>0.39881017670979807</v>
+        <v>0.35753703440000001</v>
       </c>
       <c r="F9" s="7">
         <f t="shared" si="6"/>
-        <v>1.9006748400168687</v>
+        <v>1.5194918625599636</v>
       </c>
       <c r="G9" s="7"/>
       <c r="H9" s="7">
@@ -8398,15 +8400,15 @@
       </c>
       <c r="K9" s="15">
         <f t="shared" si="9"/>
-        <v>8.3581952718295298</v>
+        <v>9.3195987016281379</v>
       </c>
       <c r="L9" s="7">
         <f t="shared" si="2"/>
-        <v>6.9859428202033516E-2</v>
+        <v>8.6854919959388863E-2</v>
       </c>
       <c r="M9" s="7">
         <f t="shared" si="3"/>
-        <v>0.4048825715636763</v>
+        <v>0.36793546728835297</v>
       </c>
       <c r="N9" s="15">
         <f t="shared" si="4"/>
@@ -8414,14 +8416,14 @@
       </c>
       <c r="O9" s="13">
         <f t="shared" si="5"/>
-        <v>500</v>
+        <v>499.81525223673225</v>
       </c>
       <c r="P9" s="21">
         <f t="shared" si="7"/>
-        <v>1250</v>
+        <v>1249.8015219624722</v>
       </c>
     </row>
-    <row r="10" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:31" x14ac:dyDescent="0.45">
       <c r="B10" s="7">
         <f t="shared" si="8"/>
         <v>3</v>
@@ -8434,11 +8436,11 @@
         <v>2.899053227347741</v>
       </c>
       <c r="E10" s="18">
-        <v>-2.8506498523888202</v>
+        <v>-4.0937250163999996</v>
       </c>
       <c r="F10" s="7">
         <f t="shared" si="6"/>
-        <v>-1.684572242541402</v>
+        <v>-3.2265355536309328</v>
       </c>
       <c r="G10" s="7"/>
       <c r="H10" s="7">
@@ -8453,15 +8455,15 @@
       </c>
       <c r="K10" s="15">
         <f t="shared" si="9"/>
-        <v>9.3085326918379643</v>
+        <v>10.07934463290812</v>
       </c>
       <c r="L10" s="7">
         <f t="shared" si="2"/>
-        <v>8.6648780875016138E-2</v>
+        <v>0.10159318822893371</v>
       </c>
       <c r="M10" s="7">
         <f t="shared" si="3"/>
-        <v>2.8519664430269036</v>
+        <v>4.0949854316949281</v>
       </c>
       <c r="N10" s="15">
         <f t="shared" si="4"/>
@@ -8469,14 +8471,14 @@
       </c>
       <c r="O10" s="13">
         <f t="shared" si="5"/>
-        <v>-3980.3051015916599</v>
+        <v>-6189.3097908979562</v>
       </c>
       <c r="P10" s="21">
         <f t="shared" si="7"/>
-        <v>1250</v>
+        <v>1249.8015219624722</v>
       </c>
     </row>
-    <row r="11" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:31" x14ac:dyDescent="0.45">
       <c r="B11" s="7">
         <f t="shared" si="8"/>
         <v>3.5</v>
@@ -8489,11 +8491,11 @@
         <v>2.899053227347741</v>
       </c>
       <c r="E11" s="18">
-        <v>-5.5973725128120009</v>
+        <v>-5.5972379218999997</v>
       </c>
       <c r="F11" s="7">
         <f t="shared" si="6"/>
-        <v>-4.131865905337099</v>
+        <v>-4.1316738412176122</v>
       </c>
       <c r="G11" s="7"/>
       <c r="H11" s="7">
@@ -8508,15 +8510,15 @@
       </c>
       <c r="K11" s="15">
         <f t="shared" si="9"/>
-        <v>8.4662465705672627</v>
+        <v>8.4660768560926538</v>
       </c>
       <c r="L11" s="7">
         <f t="shared" si="2"/>
-        <v>7.167733099364193E-2</v>
+        <v>7.1674457333267674E-2</v>
       </c>
       <c r="M11" s="7">
         <f t="shared" si="3"/>
-        <v>5.597831427165497</v>
+        <v>5.5976968104917448</v>
       </c>
       <c r="N11" s="15">
         <f t="shared" si="4"/>
@@ -8524,14 +8526,14 @@
       </c>
       <c r="O11" s="13">
         <f t="shared" si="5"/>
-        <v>-7108.3103761173097</v>
+        <v>-7107.9969642962596</v>
       </c>
       <c r="P11" s="21">
         <f t="shared" si="7"/>
-        <v>1250</v>
+        <v>1249.8015219624722</v>
       </c>
     </row>
-    <row r="12" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:31" x14ac:dyDescent="0.45">
       <c r="B12" s="7">
         <f t="shared" si="8"/>
         <v>4</v>
@@ -8544,11 +8546,11 @@
         <v>2.899053227347741</v>
       </c>
       <c r="E12" s="18">
-        <v>-5.0382954994443523</v>
+        <v>-5.0382281794999999</v>
       </c>
       <c r="F12" s="7">
         <f t="shared" si="6"/>
-        <v>-2.9585225602458056</v>
+        <v>-2.9584363767875046</v>
       </c>
       <c r="G12" s="7"/>
       <c r="H12" s="7">
@@ -8563,15 +8565,15 @@
       </c>
       <c r="K12" s="15">
         <f t="shared" si="9"/>
-        <v>6.4003136178987132</v>
+        <v>6.4002399354838477</v>
       </c>
       <c r="L12" s="7">
         <f t="shared" si="2"/>
-        <v>4.0964014407459712E-2</v>
+        <v>4.0963071231762287E-2</v>
       </c>
       <c r="M12" s="7">
         <f t="shared" si="3"/>
-        <v>5.0384620262732547</v>
+        <v>5.038394700885652</v>
       </c>
       <c r="N12" s="15">
         <f t="shared" si="4"/>
@@ -8579,14 +8581,14 @@
       </c>
       <c r="O12" s="13">
         <f t="shared" si="5"/>
-        <v>-4837.0006944137231</v>
+        <v>-4836.880379777398</v>
       </c>
       <c r="P12" s="21">
         <f t="shared" si="7"/>
-        <v>1250</v>
+        <v>1249.8015219624722</v>
       </c>
     </row>
-    <row r="13" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:31" x14ac:dyDescent="0.45">
       <c r="B13" s="7">
         <f t="shared" si="8"/>
         <v>4.5</v>
@@ -8599,11 +8601,11 @@
         <v>2.899053227347741</v>
       </c>
       <c r="E13" s="18">
-        <v>-2.7209718999853165</v>
+        <v>-2.7209796920999998</v>
       </c>
       <c r="F13" s="7">
         <f t="shared" si="6"/>
-        <v>-0.30625379486015097</v>
+        <v>-0.3062555654589319</v>
       </c>
       <c r="G13" s="7"/>
       <c r="H13" s="7">
@@ -8618,15 +8620,15 @@
       </c>
       <c r="K13" s="15">
         <f t="shared" si="9"/>
-        <v>4.9210523377758104</v>
+        <v>4.9210217470900952</v>
       </c>
       <c r="L13" s="7">
         <f t="shared" ref="L13:L27" si="11">K13^2/J13</f>
-        <v>4.8433512222257544</v>
+        <v>4.8432910070667301</v>
       </c>
       <c r="M13" s="7">
         <f t="shared" si="3"/>
-        <v>5.5553342961828509</v>
+        <v>5.5552856149755314</v>
       </c>
       <c r="N13" s="15">
         <f t="shared" si="4"/>
@@ -8634,14 +8636,14 @@
       </c>
       <c r="O13" s="13">
         <f t="shared" si="5"/>
-        <v>-2008.5067694167547</v>
+        <v>-2008.5000357321915</v>
       </c>
       <c r="P13" s="21">
         <f t="shared" si="7"/>
-        <v>1250</v>
+        <v>1249.8015219624722</v>
       </c>
     </row>
-    <row r="14" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:31" x14ac:dyDescent="0.45">
       <c r="B14" s="7">
         <f t="shared" si="8"/>
         <v>5</v>
@@ -8654,11 +8656,11 @@
         <v>2.899053227347741</v>
       </c>
       <c r="E14" s="18">
-        <v>-2.2941408826284087</v>
+        <v>-2.2941013434999999</v>
       </c>
       <c r="F14" s="7">
         <f t="shared" si="6"/>
-        <v>0.15025008462541084</v>
+        <v>0.15029562674001062</v>
       </c>
       <c r="G14" s="7"/>
       <c r="H14" s="7">
@@ -8673,15 +8675,15 @@
       </c>
       <c r="K14" s="15">
         <f t="shared" si="9"/>
-        <v>4.767925440345735</v>
+        <v>4.7678939643606295</v>
       </c>
       <c r="L14" s="7">
         <f t="shared" si="11"/>
-        <v>4.5466226009392141</v>
+        <v>4.5465625710773043</v>
       </c>
       <c r="M14" s="7">
         <f t="shared" si="3"/>
-        <v>5.092627952709516</v>
+        <v>5.0925565472530172</v>
       </c>
       <c r="N14" s="15">
         <f t="shared" si="4"/>
@@ -8689,14 +8691,14 @@
       </c>
       <c r="O14" s="13">
         <f t="shared" si="5"/>
-        <v>-1640.7439017031811</v>
+        <v>-1640.7047923957891</v>
       </c>
       <c r="P14" s="21">
         <f t="shared" si="7"/>
-        <v>1250</v>
+        <v>1249.8015219624722</v>
       </c>
     </row>
-    <row r="15" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:31" x14ac:dyDescent="0.45">
       <c r="B15" s="7">
         <f t="shared" si="8"/>
         <v>5.5</v>
@@ -8709,11 +8711,11 @@
         <v>2.899053227347741</v>
       </c>
       <c r="E15" s="18">
-        <v>0.68827144075275781</v>
+        <v>0.68823917550000002</v>
       </c>
       <c r="F15" s="7">
         <f t="shared" si="6"/>
-        <v>3.1182219085489358</v>
+        <v>3.118191329630855</v>
       </c>
       <c r="G15" s="7"/>
       <c r="H15" s="7">
@@ -8728,15 +8730,15 @@
       </c>
       <c r="K15" s="15">
         <f t="shared" si="9"/>
-        <v>4.8430504826584402</v>
+        <v>4.8430417777306349</v>
       </c>
       <c r="L15" s="7">
         <f t="shared" si="11"/>
-        <v>4.6910275955156298</v>
+        <v>4.6910107321688619</v>
       </c>
       <c r="M15" s="7">
         <f t="shared" si="3"/>
-        <v>4.7412506238380852</v>
+        <v>4.7412292553742175</v>
       </c>
       <c r="N15" s="15">
         <f t="shared" si="4"/>
@@ -8744,14 +8746,14 @@
       </c>
       <c r="O15" s="13">
         <f t="shared" si="5"/>
-        <v>500.00000000064955</v>
+        <v>499.97566200260798</v>
       </c>
       <c r="P15" s="21">
         <f t="shared" si="7"/>
-        <v>1500.0000000003247</v>
+        <v>1499.7893529637761</v>
       </c>
     </row>
-    <row r="16" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:31" x14ac:dyDescent="0.45">
       <c r="B16" s="7">
         <f t="shared" si="8"/>
         <v>6</v>
@@ -8764,11 +8766,11 @@
         <v>2.899053227347741</v>
       </c>
       <c r="E16" s="18">
-        <v>0.52065749453103116</v>
+        <v>0.52063085279999999</v>
       </c>
       <c r="F16" s="7">
         <f t="shared" si="6"/>
-        <v>2.5999573005877554</v>
+        <v>2.5999368034827359</v>
       </c>
       <c r="G16" s="7"/>
       <c r="H16" s="7">
@@ -8779,19 +8781,19 @@
         <v>5.4165984758658272</v>
       </c>
       <c r="J16" s="16">
-        <v>1000</v>
+        <v>-5</v>
       </c>
       <c r="K16" s="15">
         <f t="shared" si="9"/>
-        <v>6.4021614369329081</v>
+        <v>6.4021374425460627</v>
       </c>
       <c r="L16" s="7">
         <f t="shared" si="11"/>
-        <v>4.098767106455084E-2</v>
+        <v>-8.1974727666500478</v>
       </c>
       <c r="M16" s="7">
         <f t="shared" si="3"/>
-        <v>0.52226833695967678</v>
+        <v>8.2139890579946861</v>
       </c>
       <c r="N16" s="15">
         <f t="shared" si="4"/>
@@ -8799,14 +8801,14 @@
       </c>
       <c r="O16" s="13">
         <f t="shared" si="5"/>
-        <v>500.00000000050113</v>
+        <v>499.97254146833512</v>
       </c>
       <c r="P16" s="21">
         <f t="shared" si="7"/>
-        <v>1750.0000000005753</v>
+        <v>1749.7756236979437</v>
       </c>
     </row>
-    <row r="17" spans="2:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:19" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B17" s="7">
         <f t="shared" si="8"/>
         <v>6.5</v>
@@ -8819,11 +8821,11 @@
         <v>2.899053227347741</v>
       </c>
       <c r="E17" s="18">
-        <v>0.43278014883994498</v>
+        <v>0.43275222940000002</v>
       </c>
       <c r="F17" s="7">
         <f t="shared" si="6"/>
-        <v>2.145374137722369</v>
+        <v>2.1453567680156089</v>
       </c>
       <c r="G17" s="7"/>
       <c r="H17" s="7">
@@ -8834,19 +8836,19 @@
         <v>5.3642566000684164</v>
       </c>
       <c r="J17" s="16">
-        <v>1000</v>
+        <v>-5</v>
       </c>
       <c r="K17" s="15">
         <f t="shared" si="9"/>
-        <v>7.7021400872267858</v>
+        <v>7.7021058442874306</v>
       </c>
       <c r="L17" s="7">
         <f t="shared" si="11"/>
-        <v>5.9322961923265839E-2</v>
+        <v>-11.864486887321318</v>
       </c>
       <c r="M17" s="7">
         <f t="shared" si="3"/>
-        <v>0.43682704934707761</v>
+        <v>11.872376492997102</v>
       </c>
       <c r="N17" s="15">
         <f t="shared" si="4"/>
@@ -8854,14 +8856,14 @@
       </c>
       <c r="O17" s="13">
         <f t="shared" si="5"/>
-        <v>500.00000000041729</v>
+        <v>499.96552127852323</v>
       </c>
       <c r="P17" s="21">
         <f t="shared" si="7"/>
-        <v>2000.000000000784</v>
+        <v>1999.7583843372054</v>
       </c>
     </row>
-    <row r="18" spans="2:19" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:19" ht="15.75" x14ac:dyDescent="0.5">
       <c r="B18" s="7">
         <f t="shared" si="8"/>
         <v>7</v>
@@ -8874,11 +8876,11 @@
         <v>2.899053227347741</v>
       </c>
       <c r="E18" s="18">
-        <v>0.37987452904105873</v>
+        <v>0.37984543650000002</v>
       </c>
       <c r="F18" s="7">
         <f t="shared" si="6"/>
-        <v>1.7389759240044218</v>
+        <v>1.7389618987849647</v>
       </c>
       <c r="G18" s="7"/>
       <c r="H18" s="7">
@@ -8889,19 +8891,19 @@
         <v>4.9013230540525674</v>
       </c>
       <c r="J18" s="16">
-        <v>1000</v>
+        <v>-5</v>
       </c>
       <c r="K18" s="15">
         <f t="shared" si="9"/>
-        <v>8.7748271560879694</v>
+        <v>8.7747842282952355</v>
       </c>
       <c r="L18" s="7">
         <f t="shared" si="11"/>
-        <v>7.6997591619218875E-2</v>
+        <v>-15.399367650627763</v>
       </c>
       <c r="M18" s="7">
         <f t="shared" si="3"/>
-        <v>0.38759938974323244</v>
+        <v>15.404051629192585</v>
       </c>
       <c r="N18" s="15">
         <f t="shared" si="4"/>
@@ -8909,17 +8911,17 @@
       </c>
       <c r="O18" s="13">
         <f t="shared" si="5"/>
-        <v>500.00000000034152</v>
+        <v>499.95926180851791</v>
       </c>
       <c r="P18" s="21">
         <f t="shared" si="7"/>
-        <v>2250.000000000955</v>
+        <v>2249.7380152414644</v>
       </c>
       <c r="S18" s="14" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="19" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:19" x14ac:dyDescent="0.45">
       <c r="B19" s="7">
         <f t="shared" si="8"/>
         <v>7.5</v>
@@ -8932,11 +8934,11 @@
         <v>2.899053227347741</v>
       </c>
       <c r="E19" s="18">
-        <v>0.3456267544683212</v>
+        <v>0.34559664559999997</v>
       </c>
       <c r="F19" s="7">
         <f t="shared" si="6"/>
-        <v>1.3844236998756063</v>
+        <v>1.384412856596543</v>
       </c>
       <c r="G19" s="7"/>
       <c r="H19" s="7">
@@ -8951,15 +8953,15 @@
       </c>
       <c r="K19" s="15">
         <f t="shared" si="9"/>
-        <v>9.6443151180901801</v>
+        <v>9.6442651776877177</v>
       </c>
       <c r="L19" s="7">
         <f t="shared" si="11"/>
-        <v>9.3012814097022792E-2</v>
+        <v>9.3011850817559902E-2</v>
       </c>
       <c r="M19" s="7">
         <f t="shared" si="3"/>
-        <v>0.35792350717793392</v>
+        <v>0.35789418246526444</v>
       </c>
       <c r="N19" s="15">
         <f t="shared" si="4"/>
@@ -8967,17 +8969,17 @@
       </c>
       <c r="O19" s="13">
         <f t="shared" si="5"/>
-        <v>500.00000000029092</v>
+        <v>499.95385420286442</v>
       </c>
       <c r="P19" s="21">
         <f t="shared" si="7"/>
-        <v>2500.0000000011005</v>
+        <v>2499.7149423428964</v>
       </c>
       <c r="S19" s="2" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="20" spans="2:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:19" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B20" s="7">
         <f t="shared" si="8"/>
         <v>8</v>
@@ -8990,11 +8992,11 @@
         <v>2.899053227347741</v>
       </c>
       <c r="E20" s="18">
-        <v>0.32248097873156589</v>
+        <v>0.3224500045</v>
       </c>
       <c r="F20" s="7">
         <f t="shared" si="6"/>
-        <v>1.0846584108639115</v>
+        <v>1.0846503266206491</v>
       </c>
       <c r="G20" s="7"/>
       <c r="H20" s="7">
@@ -9009,15 +9011,15 @@
       </c>
       <c r="K20" s="15">
         <f t="shared" si="9"/>
-        <v>10.336526968027982</v>
+        <v>10.33647160598599</v>
       </c>
       <c r="L20" s="7">
         <f t="shared" si="11"/>
-        <v>0.10684378976076975</v>
+        <v>0.10684264526135459</v>
       </c>
       <c r="M20" s="7">
         <f t="shared" si="3"/>
-        <v>0.33971985083905859</v>
+        <v>0.33969008853437815</v>
       </c>
       <c r="N20" s="15">
         <f t="shared" si="4"/>
@@ -9025,18 +9027,18 @@
       </c>
       <c r="O20" s="13">
         <f t="shared" si="5"/>
-        <v>500.0000000002334</v>
+        <v>499.94929737964571</v>
       </c>
       <c r="P20" s="21">
         <f t="shared" si="7"/>
-        <v>2750.0000000012174</v>
+        <v>2749.6895910327194</v>
       </c>
       <c r="S20" s="17">
         <f>AVERAGE(K4:K35)*B35</f>
-        <v>140.49331129355255</v>
+        <v>144.93195443618953</v>
       </c>
     </row>
-    <row r="21" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:19" x14ac:dyDescent="0.45">
       <c r="B21" s="7">
         <f t="shared" si="8"/>
         <v>8.5</v>
@@ -9049,11 +9051,11 @@
         <v>2.899053227347741</v>
       </c>
       <c r="E21" s="18">
-        <v>0.30640476169421088</v>
+        <v>0.30637304510000002</v>
       </c>
       <c r="F21" s="7">
         <f>D21+E21-0.02*K21^2</f>
-        <v>0.83846775618540326</v>
+        <v>0.83846188949470202</v>
       </c>
       <c r="G21" s="7"/>
       <c r="H21" s="7">
@@ -9068,15 +9070,15 @@
       </c>
       <c r="K21" s="15">
         <f t="shared" si="9"/>
-        <v>10.878856173459939</v>
+        <v>10.878796769296315</v>
       </c>
       <c r="L21" s="7">
         <f t="shared" si="11"/>
-        <v>0.11834951164282742</v>
+        <v>0.11834821914765195</v>
       </c>
       <c r="M21" s="7">
         <f>SQRT((L21)^2+E21^2)</f>
-        <v>0.32846687031568633</v>
+        <v>0.32843681848913847</v>
       </c>
       <c r="N21" s="15">
         <f t="shared" si="4"/>
@@ -9084,14 +9086,14 @@
       </c>
       <c r="O21" s="13">
         <f t="shared" si="5"/>
-        <v>500.00000000018809</v>
+        <v>499.94551398500317</v>
       </c>
       <c r="P21" s="21">
         <f t="shared" si="7"/>
-        <v>3000.0000000013115</v>
+        <v>2999.662348025221</v>
       </c>
     </row>
-    <row r="22" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:19" x14ac:dyDescent="0.45">
       <c r="B22" s="7">
         <f t="shared" si="8"/>
         <v>9</v>
@@ -9104,11 +9106,11 @@
         <v>2.899053227347741</v>
       </c>
       <c r="E22" s="18">
-        <v>0.29503511815930472</v>
+        <v>0.29500274479999999</v>
       </c>
       <c r="F22" s="7">
         <f>D22+E22-0.02*K22^2</f>
-        <v>0.64115156924719141</v>
+        <v>0.64114736760176605</v>
       </c>
       <c r="G22" s="7"/>
       <c r="H22" s="7">
@@ -9123,15 +9125,15 @@
       </c>
       <c r="K22" s="15">
         <f t="shared" si="9"/>
-        <v>11.29809005155264</v>
+        <v>11.298027714043666</v>
       </c>
       <c r="L22" s="7">
         <f t="shared" si="11"/>
-        <v>0.12764683881299271</v>
+        <v>0.12764543022729874</v>
       </c>
       <c r="M22" s="7">
         <f t="shared" si="3"/>
-        <v>0.32146451811393595</v>
+        <v>0.32143424723797887</v>
       </c>
       <c r="N22" s="15">
         <f t="shared" si="4"/>
@@ -9139,14 +9141,14 @@
       </c>
       <c r="O22" s="13">
         <f t="shared" si="5"/>
-        <v>500.00000000014472</v>
+        <v>499.94237797040267</v>
       </c>
       <c r="P22" s="21">
         <f t="shared" si="7"/>
-        <v>3250.0000000013838</v>
+        <v>3249.6335370104225</v>
       </c>
     </row>
-    <row r="23" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:19" x14ac:dyDescent="0.45">
       <c r="B23" s="7">
         <f t="shared" si="8"/>
         <v>9.5</v>
@@ -9159,11 +9161,11 @@
         <v>2.899053227347741</v>
       </c>
       <c r="E23" s="18">
-        <v>0.2868946727906857</v>
+        <v>0.28686168490000002</v>
       </c>
       <c r="F23" s="7">
         <f t="shared" si="6"/>
-        <v>0.48607998388384965</v>
+        <v>0.48607694340783381</v>
       </c>
       <c r="G23" s="7"/>
       <c r="H23" s="7">
@@ -9178,15 +9180,15 @@
       </c>
       <c r="K23" s="15">
         <f>F22*(B23-B22) + K22</f>
-        <v>11.618665836176236</v>
+        <v>11.61860139784455</v>
       </c>
       <c r="L23" s="7">
         <f t="shared" si="11"/>
-        <v>0.13499339581272884</v>
+        <v>0.13499189844199536</v>
       </c>
       <c r="M23" s="7">
         <f t="shared" si="3"/>
-        <v>0.31706745368884315</v>
+        <v>0.31703696773190487</v>
       </c>
       <c r="N23" s="15">
         <f t="shared" si="4"/>
@@ -9194,14 +9196,14 @@
       </c>
       <c r="O23" s="13">
         <f t="shared" si="5"/>
-        <v>500.00000000011499</v>
+        <v>499.9397359750775</v>
       </c>
       <c r="P23" s="21">
         <f t="shared" si="7"/>
-        <v>3500.0000000014411</v>
+        <v>3499.6034049979612</v>
       </c>
     </row>
-    <row r="24" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:19" x14ac:dyDescent="0.45">
       <c r="B24" s="7">
         <f t="shared" si="8"/>
         <v>10</v>
@@ -9214,11 +9216,11 @@
         <v>2.899053227347741</v>
       </c>
       <c r="E24" s="18">
-        <v>0.28101635478366221</v>
+        <v>0.28098274690000002</v>
       </c>
       <c r="F24" s="7">
         <f t="shared" si="6"/>
-        <v>0.36606827907515571</v>
+        <v>0.36606596635050526</v>
       </c>
       <c r="G24" s="7"/>
       <c r="H24" s="7">
@@ -9233,15 +9235,15 @@
       </c>
       <c r="K24" s="15">
         <f t="shared" si="9"/>
-        <v>11.861705828118161</v>
+        <v>11.861639869548467</v>
       </c>
       <c r="L24" s="7">
         <f t="shared" si="11"/>
-        <v>0.14070006515281236</v>
+        <v>0.14069850039486179</v>
       </c>
       <c r="M24" s="7">
         <f t="shared" si="3"/>
-        <v>0.31427169772332786</v>
+        <v>0.31424094588202917</v>
       </c>
       <c r="N24" s="15">
         <f t="shared" si="4"/>
@@ -9249,14 +9251,14 @@
       </c>
       <c r="O24" s="13">
         <f t="shared" si="5"/>
-        <v>500.00000000008299</v>
+        <v>499.93742299264295</v>
       </c>
       <c r="P24" s="21">
         <f t="shared" si="7"/>
-        <v>3750.0000000014825</v>
+        <v>3749.5721164942825</v>
       </c>
     </row>
-    <row r="25" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:19" x14ac:dyDescent="0.45">
       <c r="B25" s="7">
         <f t="shared" si="8"/>
         <v>10.5</v>
@@ -9269,11 +9271,11 @@
         <v>2.899053227347741</v>
       </c>
       <c r="E25" s="18">
-        <v>0.2767459772718156</v>
+        <v>0.27671168730000001</v>
       </c>
       <c r="F25" s="7">
         <f t="shared" si="6"/>
-        <v>0.27428398685068522</v>
+        <v>0.27428203206494617</v>
       </c>
       <c r="G25" s="7"/>
       <c r="H25" s="7">
@@ -9288,15 +9290,15 @@
       </c>
       <c r="K25" s="15">
         <f t="shared" si="9"/>
-        <v>12.044739967655739</v>
+        <v>12.044672852723719</v>
       </c>
       <c r="L25" s="7">
         <f t="shared" si="11"/>
-        <v>0.14507576088844357</v>
+        <v>0.14507414412913974</v>
       </c>
       <c r="M25" s="7">
         <f t="shared" si="3"/>
-        <v>0.31246649793776793</v>
+        <v>0.31243537761145967</v>
       </c>
       <c r="N25" s="15">
         <f t="shared" si="4"/>
@@ -9304,14 +9306,14 @@
       </c>
       <c r="O25" s="13">
         <f t="shared" si="5"/>
-        <v>500.00000000006759</v>
+        <v>499.93526220805273</v>
       </c>
       <c r="P25" s="21">
         <f t="shared" si="7"/>
-        <v>4000.0000000015161</v>
+        <v>3999.5397475983086</v>
       </c>
     </row>
-    <row r="26" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:19" x14ac:dyDescent="0.45">
       <c r="B26" s="7">
         <f t="shared" si="8"/>
         <v>11</v>
@@ -9324,11 +9326,11 @@
         <v>2.899053227347741</v>
       </c>
       <c r="E26" s="18">
-        <v>0.27363040817363604</v>
+        <v>0.27359530310000002</v>
       </c>
       <c r="F26" s="7">
         <f t="shared" si="6"/>
-        <v>0.20471867324712356</v>
+        <v>0.20471674778732663</v>
       </c>
       <c r="G26" s="7"/>
       <c r="H26" s="7">
@@ -9339,19 +9341,19 @@
         <v>5.0941319588089202</v>
       </c>
       <c r="J26" s="16">
-        <v>1000</v>
+        <v>5</v>
       </c>
       <c r="K26" s="15">
         <f t="shared" si="9"/>
-        <v>12.181881961081082</v>
+        <v>12.181813868756192</v>
       </c>
       <c r="L26" s="7">
         <f t="shared" si="11"/>
-        <v>0.14839824811371266</v>
+        <v>29.679317826604141</v>
       </c>
       <c r="M26" s="7">
         <f t="shared" si="3"/>
-        <v>0.31128064559250979</v>
+        <v>29.680578852887297</v>
       </c>
       <c r="N26" s="15">
         <f t="shared" si="4"/>
@@ -9359,14 +9361,14 @@
       </c>
       <c r="O26" s="13">
         <f t="shared" si="5"/>
-        <v>500.00000000005053</v>
+        <v>499.93305865952016</v>
       </c>
       <c r="P26" s="21">
         <f t="shared" si="7"/>
-        <v>4250.0000000015416</v>
+        <v>4249.5062769280685</v>
       </c>
     </row>
-    <row r="27" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:19" x14ac:dyDescent="0.45">
       <c r="B27" s="7">
         <f t="shared" si="8"/>
         <v>11.5</v>
@@ -9379,11 +9381,11 @@
         <v>2.899053227347741</v>
       </c>
       <c r="E27" s="18">
-        <v>0.27135036283896757</v>
+        <v>0.27131421259999999</v>
       </c>
       <c r="F27" s="7">
         <f t="shared" si="6"/>
-        <v>0.15235190498206341</v>
+        <v>0.15234968620595746</v>
       </c>
       <c r="G27" s="7"/>
       <c r="H27" s="7">
@@ -9398,15 +9400,15 @@
       </c>
       <c r="K27" s="15">
         <f t="shared" si="9"/>
-        <v>12.284241297704643</v>
+        <v>12.284172242649856</v>
       </c>
       <c r="L27" s="7">
         <f t="shared" si="11"/>
-        <v>0.15090258426023226</v>
+        <v>0.15090088768708917</v>
       </c>
       <c r="M27" s="7">
         <f t="shared" si="3"/>
-        <v>0.31048769597079984</v>
+        <v>0.31045527836309933</v>
       </c>
       <c r="N27" s="15">
         <f t="shared" si="4"/>
@@ -9414,14 +9416,14 @@
       </c>
       <c r="O27" s="13">
         <f t="shared" si="5"/>
-        <v>500.00000000003769</v>
+        <v>499.93057791859826</v>
       </c>
       <c r="P27" s="21">
         <f t="shared" si="7"/>
-        <v>4500.0000000015607</v>
+        <v>4499.4715658873674</v>
       </c>
     </row>
-    <row r="28" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:19" x14ac:dyDescent="0.45">
       <c r="B28" s="7">
         <f t="shared" si="8"/>
         <v>12</v>
@@ -9434,11 +9436,11 @@
         <v>2.899053227347741</v>
       </c>
       <c r="E28" s="18">
-        <v>0.26967805907043779</v>
+        <v>0.26964048979999999</v>
       </c>
       <c r="F28" s="7">
         <f t="shared" si="6"/>
-        <v>0.11313299443948255</v>
+        <v>0.11313011554216912</v>
       </c>
       <c r="G28" s="7"/>
       <c r="H28" s="7">
@@ -9453,15 +9455,15 @@
       </c>
       <c r="K28" s="15">
         <f t="shared" si="9"/>
-        <v>12.360417250195674</v>
+        <v>12.360347085752835</v>
       </c>
       <c r="L28" s="7">
         <f t="shared" si="2"/>
-        <v>0.15277991459893481</v>
+        <v>0.15277818008027857</v>
       </c>
       <c r="M28" s="7">
         <f t="shared" si="3"/>
-        <v>0.30994831480241403</v>
+        <v>0.3099147722329898</v>
       </c>
       <c r="N28" s="15">
         <f t="shared" si="4"/>
@@ -9469,14 +9471,14 @@
       </c>
       <c r="O28" s="13">
         <f t="shared" si="5"/>
-        <v>500.00000000002905</v>
+        <v>499.92750634505956</v>
       </c>
       <c r="P28" s="21">
         <f t="shared" si="7"/>
-        <v>4750.0000000015752</v>
+        <v>4749.4353190598977</v>
       </c>
     </row>
-    <row r="29" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:19" x14ac:dyDescent="0.45">
       <c r="B29" s="7">
         <f t="shared" si="8"/>
         <v>12.5</v>
@@ -9489,11 +9491,11 @@
         <v>2.899053227347741</v>
       </c>
       <c r="E29" s="18">
-        <v>0.268449520522833</v>
+        <v>0.26840992600000002</v>
       </c>
       <c r="F29" s="7">
         <f t="shared" si="6"/>
-        <v>8.3873040199002435E-2</v>
+        <v>8.3869009747905121E-2</v>
       </c>
       <c r="G29" s="7"/>
       <c r="H29" s="7">
@@ -9504,19 +9506,19 @@
         <v>5.2194264374166677</v>
       </c>
       <c r="J29" s="16">
-        <v>1000</v>
+        <v>5</v>
       </c>
       <c r="K29" s="15">
         <f t="shared" si="9"/>
-        <v>12.416983747415415</v>
+        <v>12.41691214352392</v>
       </c>
       <c r="L29" s="7">
         <f t="shared" si="2"/>
-        <v>0.15418148538357856</v>
+        <v>30.835941435998357</v>
       </c>
       <c r="M29" s="7">
         <f t="shared" si="3"/>
-        <v>0.30957563777536756</v>
+        <v>30.837109594329618</v>
       </c>
       <c r="N29" s="15">
         <f t="shared" si="4"/>
@@ -9524,14 +9526,14 @@
       </c>
       <c r="O29" s="13">
         <f t="shared" si="5"/>
-        <v>500.00000000002171</v>
+        <v>499.92337043876353</v>
       </c>
       <c r="P29" s="21">
         <f t="shared" si="7"/>
-        <v>5000.0000000015862</v>
+        <v>4999.3970042792798</v>
       </c>
     </row>
-    <row r="30" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:19" x14ac:dyDescent="0.45">
       <c r="B30" s="7">
         <f t="shared" si="8"/>
         <v>13</v>
@@ -9544,11 +9546,11 @@
         <v>2.899053227347741</v>
       </c>
       <c r="E30" s="18">
-        <v>0.26754592386506326</v>
+        <v>0.26750328699999998</v>
       </c>
       <c r="F30" s="7">
         <f t="shared" si="6"/>
-        <v>6.2105266566924833E-2</v>
+        <v>6.2099318181843E-2</v>
       </c>
       <c r="G30" s="7"/>
       <c r="H30" s="7">
@@ -9563,15 +9565,15 @@
       </c>
       <c r="K30" s="15">
         <f t="shared" si="9"/>
-        <v>12.458920267514916</v>
+        <v>12.458846648397872</v>
       </c>
       <c r="L30" s="7">
         <f t="shared" si="2"/>
-        <v>0.15522469423229396</v>
+        <v>0.15522285980829489</v>
       </c>
       <c r="M30" s="7">
         <f t="shared" si="3"/>
-        <v>0.30931460857243614</v>
+        <v>0.30927680928719814</v>
       </c>
       <c r="N30" s="15">
         <f t="shared" si="4"/>
@@ -9579,14 +9581,14 @@
       </c>
       <c r="O30" s="13">
         <f t="shared" si="5"/>
-        <v>500.00000000001592</v>
+        <v>499.91736460130454</v>
       </c>
       <c r="P30" s="21">
         <f t="shared" si="7"/>
-        <v>5250.0000000015943</v>
+        <v>5249.3556865799319</v>
       </c>
     </row>
-    <row r="31" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:19" x14ac:dyDescent="0.45">
       <c r="B31" s="7">
         <f t="shared" si="8"/>
         <v>13.5</v>
@@ -9599,11 +9601,11 @@
         <v>2.899053227347741</v>
       </c>
       <c r="E31" s="18">
-        <v>0.26688074984697091</v>
+        <v>0.26683323920000002</v>
       </c>
       <c r="F31" s="7">
         <f t="shared" si="6"/>
-        <v>4.5945515941154813E-2</v>
+        <v>4.5936271111296723E-2</v>
       </c>
       <c r="G31" s="7"/>
       <c r="H31" s="7">
@@ -9618,15 +9620,15 @@
       </c>
       <c r="K31" s="15">
         <f t="shared" si="9"/>
-        <v>12.489972900798378</v>
+        <v>12.489896307488793</v>
       </c>
       <c r="L31" s="7">
         <f t="shared" si="2"/>
-        <v>0.15599942306267783</v>
+        <v>0.1559975097718222</v>
       </c>
       <c r="M31" s="7">
         <f t="shared" si="3"/>
-        <v>0.3091296728474473</v>
+        <v>0.309087690788511</v>
       </c>
       <c r="N31" s="15">
         <f t="shared" si="4"/>
@@ -9634,14 +9636,14 @@
       </c>
       <c r="O31" s="13">
         <f t="shared" si="5"/>
-        <v>500.00000000001262</v>
+        <v>499.90792334990311</v>
       </c>
       <c r="P31" s="21">
         <f t="shared" si="7"/>
-        <v>5500.0000000016007</v>
+        <v>5499.3096482548835</v>
       </c>
     </row>
-    <row r="32" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:19" x14ac:dyDescent="0.45">
       <c r="B32" s="7">
         <f t="shared" si="8"/>
         <v>14</v>
@@ -9654,11 +9656,11 @@
         <v>2.899053227347741</v>
       </c>
       <c r="E32" s="18">
-        <v>0.26639077833742736</v>
+        <v>0.26633466859999999</v>
       </c>
       <c r="F32" s="7">
         <f t="shared" si="6"/>
-        <v>3.3967824499070876E-2</v>
+        <v>3.3952364547622516E-2</v>
       </c>
       <c r="G32" s="7"/>
       <c r="H32" s="7">
@@ -9673,15 +9675,15 @@
       </c>
       <c r="K32" s="15">
         <f t="shared" si="9"/>
-        <v>12.512945658768956</v>
+        <v>12.512864443044442</v>
       </c>
       <c r="L32" s="7">
         <f t="shared" si="2"/>
-        <v>0.15657380905930487</v>
+        <v>0.1565717765700059</v>
       </c>
       <c r="M32" s="7">
         <f t="shared" si="3"/>
-        <v>0.3089974182198939</v>
+        <v>0.30894801652795845</v>
       </c>
       <c r="N32" s="15">
         <f t="shared" si="4"/>
@@ -9689,14 +9691,14 @@
       </c>
       <c r="O32" s="13">
         <f t="shared" si="5"/>
-        <v>500.00000000000927</v>
+        <v>499.89144070124473</v>
       </c>
       <c r="P32" s="21">
         <f t="shared" si="7"/>
-        <v>5750.0000000016053</v>
+        <v>5749.2553686055062</v>
       </c>
     </row>
-    <row r="33" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:18" x14ac:dyDescent="0.45">
       <c r="B33" s="7">
         <f t="shared" si="8"/>
         <v>14.5</v>
@@ -9709,11 +9711,11 @@
         <v>2.899053227347741</v>
       </c>
       <c r="E33" s="18">
-        <v>0.26602969429639273</v>
+        <v>0.26595558380000001</v>
       </c>
       <c r="F33" s="7">
         <f t="shared" si="6"/>
-        <v>2.5100220550460683E-2</v>
+        <v>2.5070689230225707E-2</v>
       </c>
       <c r="G33" s="7"/>
       <c r="H33" s="7">
@@ -9728,15 +9730,15 @@
       </c>
       <c r="K33" s="15">
         <f t="shared" si="9"/>
-        <v>12.529929571018492</v>
+        <v>12.529840625318254</v>
       </c>
       <c r="L33" s="7">
         <f t="shared" si="2"/>
-        <v>0.15699913505468366</v>
+        <v>0.15699690609587574</v>
       </c>
       <c r="M33" s="7">
         <f t="shared" si="3"/>
-        <v>0.30890213119263354</v>
+        <v>0.30883717567364855</v>
       </c>
       <c r="N33" s="15">
         <f t="shared" si="4"/>
@@ -9744,14 +9746,14 @@
       </c>
       <c r="O33" s="13">
         <f t="shared" si="5"/>
-        <v>500.00000000000711</v>
+        <v>499.85716176412097</v>
       </c>
       <c r="P33" s="21">
         <f t="shared" si="7"/>
-        <v>6000.0000000016089</v>
+        <v>5999.1839494875667</v>
       </c>
     </row>
-    <row r="34" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:18" x14ac:dyDescent="0.45">
       <c r="B34" s="7">
         <f t="shared" si="8"/>
         <v>15</v>
@@ -9764,11 +9766,11 @@
         <v>2.899053227347741</v>
       </c>
       <c r="E34" s="18">
-        <v>0.26576350275494681</v>
+        <v>0.26563357199999998</v>
       </c>
       <c r="F34" s="7">
         <f t="shared" si="6"/>
-        <v>1.854079898937E-2</v>
+        <v>1.8462899924501563E-2</v>
       </c>
       <c r="G34" s="7"/>
       <c r="H34" s="7">
@@ -9783,15 +9785,15 @@
       </c>
       <c r="K34" s="15">
         <f t="shared" si="9"/>
-        <v>12.542479681293722</v>
+        <v>12.542375969933367</v>
       </c>
       <c r="L34" s="7">
         <f t="shared" si="2"/>
-        <v>0.15731379655566588</v>
+        <v>0.15731119497116197</v>
       </c>
       <c r="M34" s="7">
         <f t="shared" si="3"/>
-        <v>0.30883307786462261</v>
+        <v>0.30871994855650986</v>
       </c>
       <c r="N34" s="15">
         <f t="shared" si="4"/>
@@ -9799,14 +9801,14 @@
       </c>
       <c r="O34" s="13">
         <f t="shared" si="5"/>
-        <v>500.00000000000529</v>
+        <v>499.75141953905472</v>
       </c>
       <c r="P34" s="21">
         <f t="shared" si="7"/>
-        <v>6250.0000000016116</v>
+        <v>6249.0596592570937</v>
       </c>
     </row>
-    <row r="35" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:18" x14ac:dyDescent="0.45">
       <c r="B35" s="7">
         <f t="shared" si="8"/>
         <v>15.5</v>
@@ -9819,11 +9821,11 @@
         <v>2.899053227347741</v>
       </c>
       <c r="E35" s="18">
-        <v>0</v>
+        <v>-1.6307550583999999</v>
       </c>
       <c r="F35" s="7">
         <f t="shared" si="6"/>
-        <v>-0.25187537446369479</v>
+        <v>-1.8825588075158335</v>
       </c>
       <c r="G35" s="7"/>
       <c r="H35" s="7">
@@ -9838,15 +9840,15 @@
       </c>
       <c r="K35" s="15">
         <f t="shared" si="9"/>
-        <v>12.551750080788407</v>
+        <v>12.551607419895618</v>
       </c>
       <c r="L35" s="7">
         <f t="shared" si="2"/>
-        <v>0.15754643009057179</v>
+        <v>0.15754284882317873</v>
       </c>
       <c r="M35" s="7">
         <f t="shared" si="3"/>
-        <v>0.15754643009057179</v>
+        <v>1.6383472799478473</v>
       </c>
       <c r="N35" s="15">
         <f t="shared" si="4"/>
@@ -9854,18 +9856,18 @@
       </c>
       <c r="O35" s="13">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>-3070.2895936568625</v>
       </c>
       <c r="P35" s="21">
         <f t="shared" si="7"/>
-        <v>6250.0000000016116</v>
+        <v>6249.0596592570937</v>
       </c>
     </row>
-    <row r="39" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:18" x14ac:dyDescent="0.45">
       <c r="Q39" s="7"/>
       <c r="R39" s="7"/>
     </row>
-    <row r="40" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:18" x14ac:dyDescent="0.45">
       <c r="Q40" s="7"/>
       <c r="R40" s="7"/>
     </row>
@@ -9906,9 +9908,9 @@
       <selection activeCell="D84" sqref="D84"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData>
-    <row r="1" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A1" s="1" t="s">
         <v>18</v>
       </c>
@@ -9917,7 +9919,7 @@
         <v>68.556546004010443</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A2" s="3" t="s">
         <v>15</v>
       </c>
@@ -9932,7 +9934,7 @@
         <v>68.556546004010443</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A3" s="6">
         <v>0</v>
       </c>
@@ -9949,7 +9951,7 @@
         <v>68.556546004010443</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A4" s="6">
         <f>2*3.14/31</f>
         <v>0.20258064516129032</v>
@@ -9968,7 +9970,7 @@
         <v>68.556546004010443</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A5" s="6">
         <f t="shared" ref="A5:A34" si="2">0.2025+A4</f>
         <v>0.40508064516129033</v>
@@ -9987,7 +9989,7 @@
         <v>68.556546004010443</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A6" s="6">
         <f t="shared" si="2"/>
         <v>0.6075806451612904</v>
@@ -10006,7 +10008,7 @@
         <v>68.556546004010443</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A7" s="6">
         <f t="shared" si="2"/>
         <v>0.81008064516129041</v>
@@ -10025,7 +10027,7 @@
         <v>68.556546004010443</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A8" s="6">
         <f t="shared" si="2"/>
         <v>1.0125806451612904</v>
@@ -10044,7 +10046,7 @@
         <v>68.556546004010443</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A9" s="6">
         <f t="shared" si="2"/>
         <v>1.2150806451612906</v>
@@ -10063,7 +10065,7 @@
         <v>68.556546004010443</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A10" s="6">
         <f t="shared" si="2"/>
         <v>1.4175806451612907</v>
@@ -10082,7 +10084,7 @@
         <v>4.8476798574163293</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A11" s="6">
         <f t="shared" si="2"/>
         <v>1.6200806451612908</v>
@@ -10101,7 +10103,7 @@
         <v>4.8476798574163293</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A12" s="6">
         <f t="shared" si="2"/>
         <v>1.8225806451612909</v>
@@ -10120,7 +10122,7 @@
         <v>4.8476798574163293</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A13" s="6">
         <f t="shared" si="2"/>
         <v>2.025080645161291</v>
@@ -10134,12 +10136,12 @@
         <v>5.39145187928181</v>
       </c>
       <c r="D13" s="7"/>
-      <c r="M13">
+      <c r="M13" t="e">
         <f>SQRT(4.7*Sheet1!J16)</f>
-        <v>68.556546004010443</v>
+        <v>#NUM!</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A14" s="6">
         <f t="shared" si="2"/>
         <v>2.2275806451612912</v>
@@ -10153,12 +10155,12 @@
         <v>4.7517583932179228</v>
       </c>
       <c r="D14" s="7"/>
-      <c r="M14">
+      <c r="M14" t="e">
         <f>SQRT(4.7*Sheet1!J17)</f>
-        <v>68.556546004010443</v>
+        <v>#NUM!</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A15" s="6">
         <f t="shared" si="2"/>
         <v>2.4300806451612913</v>
@@ -10172,12 +10174,12 @@
         <v>3.9178780501913151</v>
       </c>
       <c r="D15" s="7"/>
-      <c r="M15">
+      <c r="M15" t="e">
         <f>SQRT(4.7*Sheet1!J18)</f>
-        <v>68.556546004010443</v>
+        <v>#NUM!</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A16" s="6">
         <f t="shared" si="2"/>
         <v>2.6325806451612914</v>
@@ -10196,7 +10198,7 @@
         <v>68.556546004010443</v>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A17" s="6">
         <f t="shared" si="2"/>
         <v>2.8350806451612915</v>
@@ -10215,7 +10217,7 @@
         <v>68.556546004010443</v>
       </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A18" s="6">
         <f t="shared" si="2"/>
         <v>3.0375806451612917</v>
@@ -10234,7 +10236,7 @@
         <v>68.556546004010443</v>
       </c>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A19" s="6">
         <f t="shared" si="2"/>
         <v>3.2400806451612918</v>
@@ -10253,7 +10255,7 @@
         <v>68.556546004010443</v>
       </c>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A20" s="6">
         <f t="shared" si="2"/>
         <v>3.4425806451612919</v>
@@ -10272,7 +10274,7 @@
         <v>68.556546004010443</v>
       </c>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A21" s="6">
         <f t="shared" si="2"/>
         <v>3.645080645161292</v>
@@ -10291,7 +10293,7 @@
         <v>68.556546004010443</v>
       </c>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A22" s="6">
         <f t="shared" si="2"/>
         <v>3.8475806451612922</v>
@@ -10310,7 +10312,7 @@
         <v>68.556546004010443</v>
       </c>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A23" s="6">
         <f t="shared" si="2"/>
         <v>4.0500806451612918</v>
@@ -10326,10 +10328,10 @@
       <c r="D23" s="7"/>
       <c r="M23">
         <f>SQRT(4.7*Sheet1!J26)</f>
-        <v>68.556546004010443</v>
+        <v>4.8476798574163293</v>
       </c>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A24" s="6">
         <f t="shared" si="2"/>
         <v>4.2525806451612915</v>
@@ -10348,7 +10350,7 @@
         <v>68.556546004010443</v>
       </c>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A25" s="6">
         <f t="shared" si="2"/>
         <v>4.4550806451612912</v>
@@ -10367,7 +10369,7 @@
         <v>68.556546004010443</v>
       </c>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A26" s="6">
         <f t="shared" si="2"/>
         <v>4.6575806451612909</v>
@@ -10383,10 +10385,10 @@
       <c r="D26" s="7"/>
       <c r="M26">
         <f>SQRT(4.7*Sheet1!J29)</f>
-        <v>68.556546004010443</v>
+        <v>4.8476798574163293</v>
       </c>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A27" s="6">
         <f t="shared" si="2"/>
         <v>4.8600806451612906</v>
@@ -10405,7 +10407,7 @@
         <v>68.556546004010443</v>
       </c>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A28" s="6">
         <f t="shared" si="2"/>
         <v>5.0625806451612902</v>
@@ -10424,7 +10426,7 @@
         <v>68.556546004010443</v>
       </c>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A29" s="6">
         <f t="shared" si="2"/>
         <v>5.2650806451612899</v>
@@ -10443,7 +10445,7 @@
         <v>68.556546004010443</v>
       </c>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A30" s="6">
         <f t="shared" si="2"/>
         <v>5.4675806451612896</v>
@@ -10462,7 +10464,7 @@
         <v>68.556546004010443</v>
       </c>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A31" s="6">
         <f t="shared" si="2"/>
         <v>5.6700806451612893</v>
@@ -10481,7 +10483,7 @@
         <v>68.556546004010443</v>
       </c>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A32" s="6">
         <f t="shared" si="2"/>
         <v>5.872580645161289</v>
@@ -10500,7 +10502,7 @@
         <v>68.556546004010443</v>
       </c>
     </row>
-    <row r="33" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:13" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A33" s="6">
         <f t="shared" si="2"/>
         <v>6.0750806451612887</v>
@@ -10515,7 +10517,7 @@
       </c>
       <c r="D33" s="7"/>
     </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A34" s="6">
         <f t="shared" si="2"/>
         <v>6.2775806451612883</v>
@@ -10533,200 +10535,200 @@
         <v>12</v>
       </c>
     </row>
-    <row r="35" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:13" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A35" s="9"/>
       <c r="B35" s="10"/>
       <c r="C35" s="11"/>
       <c r="D35" s="7"/>
       <c r="M35" s="8">
         <f>-Sheet1!E4</f>
-        <v>0.89905322734774096</v>
+        <v>-5.3622772123000004</v>
       </c>
     </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:13" x14ac:dyDescent="0.45">
       <c r="M36" s="8">
         <f>-Sheet1!E5</f>
-        <v>-3.3333333333333335</v>
+        <v>-0.80693497749999998</v>
       </c>
     </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:13" x14ac:dyDescent="0.45">
       <c r="M37" s="8">
         <f>-Sheet1!E6</f>
-        <v>-0.81178188793316886</v>
+        <v>-0.57338012189999998</v>
       </c>
     </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:13" x14ac:dyDescent="0.45">
       <c r="M38" s="8">
         <f>-Sheet1!E7</f>
-        <v>-0.57540684173199919</v>
+        <v>-0.46218115119999997</v>
       </c>
     </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:13" x14ac:dyDescent="0.45">
       <c r="M39" s="8">
         <f>-Sheet1!E8</f>
-        <v>-0.46330762212964116</v>
+        <v>-0.39808266819999999</v>
       </c>
     </row>
-    <row r="40" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:13" x14ac:dyDescent="0.45">
       <c r="M40" s="8">
         <f>-Sheet1!E9</f>
-        <v>-0.39881017670979807</v>
+        <v>-0.35753703440000001</v>
       </c>
     </row>
-    <row r="41" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:13" x14ac:dyDescent="0.45">
       <c r="M41" s="8">
         <f>-Sheet1!E10</f>
-        <v>2.8506498523888202</v>
+        <v>4.0937250163999996</v>
       </c>
     </row>
-    <row r="42" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:13" x14ac:dyDescent="0.45">
       <c r="M42" s="8">
         <f>-Sheet1!E11</f>
-        <v>5.5973725128120009</v>
+        <v>5.5972379218999997</v>
       </c>
     </row>
-    <row r="43" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:13" x14ac:dyDescent="0.45">
       <c r="M43" s="8">
         <f>-Sheet1!E12</f>
-        <v>5.0382954994443523</v>
+        <v>5.0382281794999999</v>
       </c>
     </row>
-    <row r="44" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:13" x14ac:dyDescent="0.45">
       <c r="M44" s="8">
         <f>-Sheet1!E13</f>
-        <v>2.7209718999853165</v>
+        <v>2.7209796920999998</v>
       </c>
     </row>
-    <row r="45" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:13" x14ac:dyDescent="0.45">
       <c r="M45" s="8">
         <f>-Sheet1!E14</f>
-        <v>2.2941408826284087</v>
+        <v>2.2941013434999999</v>
       </c>
     </row>
-    <row r="46" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:13" x14ac:dyDescent="0.45">
       <c r="M46" s="8">
         <f>-Sheet1!E15</f>
-        <v>-0.68827144075275781</v>
+        <v>-0.68823917550000002</v>
       </c>
     </row>
-    <row r="47" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:13" x14ac:dyDescent="0.45">
       <c r="M47" s="8">
         <f>-Sheet1!E16</f>
-        <v>-0.52065749453103116</v>
+        <v>-0.52063085279999999</v>
       </c>
     </row>
-    <row r="48" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:13" x14ac:dyDescent="0.45">
       <c r="M48" s="8">
         <f>-Sheet1!E17</f>
-        <v>-0.43278014883994498</v>
+        <v>-0.43275222940000002</v>
       </c>
     </row>
-    <row r="49" spans="13:13" x14ac:dyDescent="0.25">
+    <row r="49" spans="13:13" x14ac:dyDescent="0.45">
       <c r="M49" s="8">
         <f>-Sheet1!E18</f>
-        <v>-0.37987452904105873</v>
+        <v>-0.37984543650000002</v>
       </c>
     </row>
-    <row r="50" spans="13:13" x14ac:dyDescent="0.25">
+    <row r="50" spans="13:13" x14ac:dyDescent="0.45">
       <c r="M50" s="8">
         <f>-Sheet1!E19</f>
-        <v>-0.3456267544683212</v>
+        <v>-0.34559664559999997</v>
       </c>
     </row>
-    <row r="51" spans="13:13" x14ac:dyDescent="0.25">
+    <row r="51" spans="13:13" x14ac:dyDescent="0.45">
       <c r="M51" s="8">
         <f>-Sheet1!E20</f>
-        <v>-0.32248097873156589</v>
+        <v>-0.3224500045</v>
       </c>
     </row>
-    <row r="52" spans="13:13" x14ac:dyDescent="0.25">
+    <row r="52" spans="13:13" x14ac:dyDescent="0.45">
       <c r="M52" s="8">
         <f>-Sheet1!E21</f>
-        <v>-0.30640476169421088</v>
+        <v>-0.30637304510000002</v>
       </c>
     </row>
-    <row r="53" spans="13:13" x14ac:dyDescent="0.25">
+    <row r="53" spans="13:13" x14ac:dyDescent="0.45">
       <c r="M53" s="8">
         <f>-Sheet1!E22</f>
-        <v>-0.29503511815930472</v>
+        <v>-0.29500274479999999</v>
       </c>
     </row>
-    <row r="54" spans="13:13" x14ac:dyDescent="0.25">
+    <row r="54" spans="13:13" x14ac:dyDescent="0.45">
       <c r="M54" s="8">
         <f>-Sheet1!E23</f>
-        <v>-0.2868946727906857</v>
+        <v>-0.28686168490000002</v>
       </c>
     </row>
-    <row r="55" spans="13:13" x14ac:dyDescent="0.25">
+    <row r="55" spans="13:13" x14ac:dyDescent="0.45">
       <c r="M55" s="8">
         <f>-Sheet1!E24</f>
-        <v>-0.28101635478366221</v>
+        <v>-0.28098274690000002</v>
       </c>
     </row>
-    <row r="56" spans="13:13" x14ac:dyDescent="0.25">
+    <row r="56" spans="13:13" x14ac:dyDescent="0.45">
       <c r="M56" s="8">
         <f>-Sheet1!E25</f>
-        <v>-0.2767459772718156</v>
+        <v>-0.27671168730000001</v>
       </c>
     </row>
-    <row r="57" spans="13:13" x14ac:dyDescent="0.25">
+    <row r="57" spans="13:13" x14ac:dyDescent="0.45">
       <c r="M57" s="8">
         <f>-Sheet1!E26</f>
-        <v>-0.27363040817363604</v>
+        <v>-0.27359530310000002</v>
       </c>
     </row>
-    <row r="58" spans="13:13" x14ac:dyDescent="0.25">
+    <row r="58" spans="13:13" x14ac:dyDescent="0.45">
       <c r="M58" s="8">
         <f>-Sheet1!E27</f>
-        <v>-0.27135036283896757</v>
+        <v>-0.27131421259999999</v>
       </c>
     </row>
-    <row r="59" spans="13:13" x14ac:dyDescent="0.25">
+    <row r="59" spans="13:13" x14ac:dyDescent="0.45">
       <c r="M59" s="8">
         <f>-Sheet1!E28</f>
-        <v>-0.26967805907043779</v>
+        <v>-0.26964048979999999</v>
       </c>
     </row>
-    <row r="60" spans="13:13" x14ac:dyDescent="0.25">
+    <row r="60" spans="13:13" x14ac:dyDescent="0.45">
       <c r="M60" s="8">
         <f>-Sheet1!E29</f>
-        <v>-0.268449520522833</v>
+        <v>-0.26840992600000002</v>
       </c>
     </row>
-    <row r="61" spans="13:13" x14ac:dyDescent="0.25">
+    <row r="61" spans="13:13" x14ac:dyDescent="0.45">
       <c r="M61" s="8">
         <f>-Sheet1!E30</f>
-        <v>-0.26754592386506326</v>
+        <v>-0.26750328699999998</v>
       </c>
     </row>
-    <row r="62" spans="13:13" x14ac:dyDescent="0.25">
+    <row r="62" spans="13:13" x14ac:dyDescent="0.45">
       <c r="M62" s="8">
         <f>-Sheet1!E31</f>
-        <v>-0.26688074984697091</v>
+        <v>-0.26683323920000002</v>
       </c>
     </row>
-    <row r="63" spans="13:13" x14ac:dyDescent="0.25">
+    <row r="63" spans="13:13" x14ac:dyDescent="0.45">
       <c r="M63" s="8">
         <f>-Sheet1!E32</f>
-        <v>-0.26639077833742736</v>
+        <v>-0.26633466859999999</v>
       </c>
     </row>
-    <row r="64" spans="13:13" x14ac:dyDescent="0.25">
+    <row r="64" spans="13:13" x14ac:dyDescent="0.45">
       <c r="M64" s="8">
         <f>-Sheet1!E33</f>
-        <v>-0.26602969429639273</v>
+        <v>-0.26595558380000001</v>
       </c>
     </row>
-    <row r="65" spans="13:13" x14ac:dyDescent="0.25">
+    <row r="65" spans="13:13" x14ac:dyDescent="0.45">
       <c r="M65" s="8">
         <f>-Sheet1!E34</f>
-        <v>-0.26576350275494681</v>
+        <v>-0.26563357199999998</v>
       </c>
     </row>
-    <row r="66" spans="13:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="66" spans="13:13" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="M66" s="11">
         <f>-Sheet1!E35</f>
-        <v>0</v>
+        <v>1.6307550583999999</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated to optimize last rider input
</commit_message>
<xml_diff>
--- a/optimize 1.xlsx
+++ b/optimize 1.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mackr\OneDrive\Desktop\solver\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Chris\PycharmProjects\ride_solver\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D02E210-6711-4B9B-83DB-F74777721145}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2B02698-7E66-441B-9D9E-B1705074F3BC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="22695" windowHeight="14595" xr2:uid="{D30F47EA-90C8-427E-9981-7FBDEA5670DF}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{D30F47EA-90C8-427E-9981-7FBDEA5670DF}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -70,9 +70,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -929,88 +927,88 @@
                   <c:v>0.81178188793316886</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.57540684173199907</c:v>
+                  <c:v>0.57540684173199919</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.46330762212964111</c:v>
+                  <c:v>0.46330762212964116</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>0.39881017670979807</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>-2.8506498523458927</c:v>
+                  <c:v>-2.8506498523888202</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>-5.5973725128120062</c:v>
+                  <c:v>-5.5973725128120009</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>-5.0382954994443567</c:v>
+                  <c:v>-5.0382954994443523</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>-2.720971899993581</c:v>
+                  <c:v>-2.7209718999853165</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>-2.294140882637894</c:v>
+                  <c:v>-2.2941408826284087</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.68827144075126734</c:v>
+                  <c:v>0.68827144075275781</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.52065749453026178</c:v>
+                  <c:v>0.52065749453103116</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0.43278014883945631</c:v>
+                  <c:v>0.43278014883994498</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0.37987491510003324</c:v>
+                  <c:v>0.37987452904105873</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0.3456269606042266</c:v>
+                  <c:v>0.3456267544683212</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0.32248109840558953</c:v>
+                  <c:v>0.32248097873156589</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0.30640483555087467</c:v>
+                  <c:v>0.30640476169421088</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>0.2950351658610682</c:v>
+                  <c:v>0.29503511815930472</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>0.2868947046668639</c:v>
+                  <c:v>0.2868946727906857</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>0.28101637663437412</c:v>
+                  <c:v>0.28101635478366221</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>0.27674599253790766</c:v>
+                  <c:v>0.2767459772718156</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>0.27363041899152879</c:v>
+                  <c:v>0.27363040817363604</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>0.27135037058589395</c:v>
+                  <c:v>0.27135036283896757</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>0.26967806466165845</c:v>
+                  <c:v>0.26967805907043779</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>0.26844952458160359</c:v>
+                  <c:v>0.268449520522833</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>0.26754592682403278</c:v>
+                  <c:v>0.26754592386506326</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>0.2668807520109866</c:v>
+                  <c:v>0.26688074984697091</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>0.26639077992376387</c:v>
+                  <c:v>0.26639077833742736</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>0.26602969546127081</c:v>
+                  <c:v>0.26602969429639273</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>0.26576350361143186</c:v>
+                  <c:v>0.26576350275494681</c:v>
                 </c:pt>
                 <c:pt idx="31">
                   <c:v>0</c:v>
@@ -1183,91 +1181,91 @@
                   <c:v>0.81195696988029709</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.57638462148486058</c:v>
+                  <c:v>0.57638462148486069</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.46619025145351362</c:v>
+                  <c:v>0.46619025145351367</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>0.4048825715636763</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>2.8519664429839962</c:v>
+                  <c:v>2.8519664430269036</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>5.5978314271655067</c:v>
+                  <c:v>5.597831427165497</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>5.0384620262732609</c:v>
+                  <c:v>5.0384620262732547</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>5.5553342962135712</c:v>
+                  <c:v>5.5553342961828509</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>5.0926279527306129</c:v>
+                  <c:v>5.092627952709516</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>4.7412506238459109</c:v>
+                  <c:v>4.7412506238380852</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.52226833695891284</c:v>
+                  <c:v>0.52226833695967678</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0.43682704934659822</c:v>
+                  <c:v>0.43682704934707761</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0.38759976810806013</c:v>
+                  <c:v>0.38759938974323244</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0.35792370719944266</c:v>
+                  <c:v>0.35792350717793392</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0.33971996612339145</c:v>
+                  <c:v>0.33971985083905859</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0.3284669412905612</c:v>
+                  <c:v>0.32846687031568633</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>0.32146456408689461</c:v>
+                  <c:v>0.32146451811393595</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>0.31706748463930701</c:v>
+                  <c:v>0.31706745368884315</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>0.31427171916803981</c:v>
+                  <c:v>0.31427169772332786</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>0.31246651311198287</c:v>
+                  <c:v>0.31246649793776793</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>0.31128065649395015</c:v>
+                  <c:v>0.31128064559250979</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>0.3104877038881822</c:v>
+                  <c:v>0.31048769597079984</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>0.3099483205972931</c:v>
+                  <c:v>0.30994831480241403</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>0.30957564204020505</c:v>
+                  <c:v>0.30957563777536756</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>0.30931461172357011</c:v>
+                  <c:v>0.30931460857243614</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>0.30912967518223977</c:v>
+                  <c:v>0.3091296728474473</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>0.30899741995329605</c:v>
+                  <c:v>0.3089974182198939</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>0.30890213248139958</c:v>
+                  <c:v>0.30890213119263354</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>0.3088330788237969</c:v>
+                  <c:v>0.30883307786462261</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>0.15754643042825731</c:v>
+                  <c:v>0.15754643009057179</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1429,7 +1427,7 @@
                   <c:v>3.3558879186470741E-2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>5.1762900101017813E-2</c:v>
+                  <c:v>5.1762900101017827E-2</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>6.9859428202033516E-2</c:v>
@@ -1438,79 +1436,79 @@
                   <c:v>8.6648780875016138E-2</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>7.1677330994005375E-2</c:v>
+                  <c:v>7.167733099364193E-2</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>4.0964014407687904E-2</c:v>
+                  <c:v>4.0964014407459712E-2</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>4.8433512222563468</c:v>
+                  <c:v>4.8433512222257544</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>4.5466226009580577</c:v>
+                  <c:v>4.5466226009392141</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>4.6910275955237584</c:v>
+                  <c:v>4.6910275955156298</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>4.0987671064589809E-2</c:v>
+                  <c:v>4.098767106455084E-2</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>5.9322961923300797E-2</c:v>
+                  <c:v>5.9322961923265839E-2</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>7.699759161924831E-2</c:v>
+                  <c:v>7.6997591619218875E-2</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>9.3012817820323904E-2</c:v>
+                  <c:v>9.3012814097022792E-2</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0.10684379511231673</c:v>
+                  <c:v>0.10684378976076975</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0.11834951741269768</c:v>
+                  <c:v>0.11834951164282742</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>0.127646844335883</c:v>
+                  <c:v>0.12764683881299271</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>0.13499340076318592</c:v>
+                  <c:v>0.13499339581272884</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>0.14070006941051191</c:v>
+                  <c:v>0.14070006515281236</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>0.14507576444937076</c:v>
+                  <c:v>0.14507576088844357</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>0.14839825103357857</c:v>
+                  <c:v>0.14839824811371266</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>0.15090258662015546</c:v>
+                  <c:v>0.15090258426023226</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>0.15277991648585471</c:v>
+                  <c:v>0.15277991459893481</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>0.15418148687996286</c:v>
+                  <c:v>0.15418148538357856</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>0.15522469541143333</c:v>
+                  <c:v>0.15522469423229396</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>0.15599942398716518</c:v>
+                  <c:v>0.15599942306267783</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>0.15657380978120963</c:v>
+                  <c:v>0.15657380905930487</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>0.15699913561653658</c:v>
+                  <c:v>0.15699913505468366</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>0.15731379699175144</c:v>
+                  <c:v>0.15731379655566588</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>0.15754643042825731</c:v>
+                  <c:v>0.15754643009057179</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1681,7 +1679,7 @@
                   <c:v>5.7930026054258548</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>7.1946438481010171</c:v>
+                  <c:v>7.194643848101018</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>8.3581952718295298</c:v>
@@ -1690,79 +1688,79 @@
                   <c:v>9.3085326918379643</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>8.4662465705887264</c:v>
+                  <c:v>8.4662465705672627</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>6.4003136179165399</c:v>
+                  <c:v>6.4003136178987132</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>4.9210523377913526</c:v>
+                  <c:v>4.9210523377758104</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>4.7679254403556151</c:v>
+                  <c:v>4.767925440345735</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>4.8430504826626359</c:v>
+                  <c:v>4.8430504826584402</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>6.4021614369359519</c:v>
+                  <c:v>6.4021614369329081</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>7.7021400872290551</c:v>
+                  <c:v>7.7021400872267858</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>8.7748271560896463</c:v>
+                  <c:v>8.7748271560879694</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>9.6443153111210496</c:v>
+                  <c:v>9.6443151180901801</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>10.336527226893795</c:v>
+                  <c:v>10.336526968027982</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>10.878856438647293</c:v>
+                  <c:v>10.878856173459939</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>11.298090295969624</c:v>
+                  <c:v>11.29809005155264</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>11.618666049215198</c:v>
+                  <c:v>11.618665836176236</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>11.861706007590641</c:v>
+                  <c:v>11.861705828118161</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>12.044740115476579</c:v>
+                  <c:v>12.044739967655739</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>12.181882080925696</c:v>
+                  <c:v>12.181881961081082</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>12.284241393759546</c:v>
+                  <c:v>12.284241297704643</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>12.360417326524809</c:v>
+                  <c:v>12.360417250195674</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>12.416983807670961</c:v>
+                  <c:v>12.416983747415415</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>12.458920314836005</c:v>
+                  <c:v>12.458920267514916</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>12.489972937807559</c:v>
+                  <c:v>12.489972900798378</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>12.512945687615272</c:v>
+                  <c:v>12.512945658768956</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>12.529929593438927</c:v>
+                  <c:v>12.529929571018492</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>12.542479698678067</c:v>
+                  <c:v>12.542479681293722</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>12.551750094240138</c:v>
+                  <c:v>12.551750080788407</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2842,7 +2840,7 @@
                   <c:v>3.3558879186470741E-2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>5.1762900101017813E-2</c:v>
+                  <c:v>5.1762900101017827E-2</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>6.9859428202033516E-2</c:v>
@@ -2851,79 +2849,79 @@
                   <c:v>8.6648780875016138E-2</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>7.1677330994005375E-2</c:v>
+                  <c:v>7.167733099364193E-2</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>4.0964014407687904E-2</c:v>
+                  <c:v>4.0964014407459712E-2</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>4.8433512222563468</c:v>
+                  <c:v>4.8433512222257544</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>4.5466226009580577</c:v>
+                  <c:v>4.5466226009392141</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>4.6910275955237584</c:v>
+                  <c:v>4.6910275955156298</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>4.0987671064589809E-2</c:v>
+                  <c:v>4.098767106455084E-2</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>5.9322961923300797E-2</c:v>
+                  <c:v>5.9322961923265839E-2</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>7.699759161924831E-2</c:v>
+                  <c:v>7.6997591619218875E-2</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>9.3012817820323904E-2</c:v>
+                  <c:v>9.3012814097022792E-2</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0.10684379511231673</c:v>
+                  <c:v>0.10684378976076975</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0.11834951741269768</c:v>
+                  <c:v>0.11834951164282742</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>0.127646844335883</c:v>
+                  <c:v>0.12764683881299271</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>0.13499340076318592</c:v>
+                  <c:v>0.13499339581272884</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>0.14070006941051191</c:v>
+                  <c:v>0.14070006515281236</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>0.14507576444937076</c:v>
+                  <c:v>0.14507576088844357</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>0.14839825103357857</c:v>
+                  <c:v>0.14839824811371266</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>0.15090258662015546</c:v>
+                  <c:v>0.15090258426023226</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>0.15277991648585471</c:v>
+                  <c:v>0.15277991459893481</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>0.15418148687996286</c:v>
+                  <c:v>0.15418148538357856</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>0.15522469541143333</c:v>
+                  <c:v>0.15522469423229396</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>0.15599942398716518</c:v>
+                  <c:v>0.15599942306267783</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>0.15657380978120963</c:v>
+                  <c:v>0.15657380905930487</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>0.15699913561653658</c:v>
+                  <c:v>0.15699913505468366</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>0.15731379699175144</c:v>
+                  <c:v>0.15731379655566588</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>0.15754643042825731</c:v>
+                  <c:v>0.15754643009057179</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2944,88 +2942,88 @@
                   <c:v>0.81178188793316886</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.57540684173199907</c:v>
+                  <c:v>0.57540684173199919</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.46330762212964111</c:v>
+                  <c:v>0.46330762212964116</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>0.39881017670979807</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>-2.8506498523458927</c:v>
+                  <c:v>-2.8506498523888202</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>-5.5973725128120062</c:v>
+                  <c:v>-5.5973725128120009</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>-5.0382954994443567</c:v>
+                  <c:v>-5.0382954994443523</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>-2.720971899993581</c:v>
+                  <c:v>-2.7209718999853165</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>-2.294140882637894</c:v>
+                  <c:v>-2.2941408826284087</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.68827144075126734</c:v>
+                  <c:v>0.68827144075275781</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.52065749453026178</c:v>
+                  <c:v>0.52065749453103116</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0.43278014883945631</c:v>
+                  <c:v>0.43278014883994498</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0.37987491510003324</c:v>
+                  <c:v>0.37987452904105873</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0.3456269606042266</c:v>
+                  <c:v>0.3456267544683212</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0.32248109840558953</c:v>
+                  <c:v>0.32248097873156589</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0.30640483555087467</c:v>
+                  <c:v>0.30640476169421088</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>0.2950351658610682</c:v>
+                  <c:v>0.29503511815930472</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>0.2868947046668639</c:v>
+                  <c:v>0.2868946727906857</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>0.28101637663437412</c:v>
+                  <c:v>0.28101635478366221</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>0.27674599253790766</c:v>
+                  <c:v>0.2767459772718156</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>0.27363041899152879</c:v>
+                  <c:v>0.27363040817363604</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>0.27135037058589395</c:v>
+                  <c:v>0.27135036283896757</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>0.26967806466165845</c:v>
+                  <c:v>0.26967805907043779</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>0.26844952458160359</c:v>
+                  <c:v>0.268449520522833</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>0.26754592682403278</c:v>
+                  <c:v>0.26754592386506326</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>0.2668807520109866</c:v>
+                  <c:v>0.26688074984697091</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>0.26639077992376387</c:v>
+                  <c:v>0.26639077833742736</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>0.26602969546127081</c:v>
+                  <c:v>0.26602969429639273</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>0.26576350361143186</c:v>
+                  <c:v>0.26576350275494681</c:v>
                 </c:pt>
                 <c:pt idx="31">
                   <c:v>0</c:v>
@@ -3831,88 +3829,88 @@
                   <c:v>-0.81178188793316886</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>-0.57540684173199907</c:v>
+                  <c:v>-0.57540684173199919</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>-0.46330762212964111</c:v>
+                  <c:v>-0.46330762212964116</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>-0.39881017670979807</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>2.8506498523458927</c:v>
+                  <c:v>2.8506498523888202</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>5.5973725128120062</c:v>
+                  <c:v>5.5973725128120009</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>5.0382954994443567</c:v>
+                  <c:v>5.0382954994443523</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>2.720971899993581</c:v>
+                  <c:v>2.7209718999853165</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>2.294140882637894</c:v>
+                  <c:v>2.2941408826284087</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>-0.68827144075126734</c:v>
+                  <c:v>-0.68827144075275781</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>-0.52065749453026178</c:v>
+                  <c:v>-0.52065749453103116</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>-0.43278014883945631</c:v>
+                  <c:v>-0.43278014883994498</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>-0.37987491510003324</c:v>
+                  <c:v>-0.37987452904105873</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>-0.3456269606042266</c:v>
+                  <c:v>-0.3456267544683212</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>-0.32248109840558953</c:v>
+                  <c:v>-0.32248097873156589</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>-0.30640483555087467</c:v>
+                  <c:v>-0.30640476169421088</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>-0.2950351658610682</c:v>
+                  <c:v>-0.29503511815930472</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>-0.2868947046668639</c:v>
+                  <c:v>-0.2868946727906857</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>-0.28101637663437412</c:v>
+                  <c:v>-0.28101635478366221</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>-0.27674599253790766</c:v>
+                  <c:v>-0.2767459772718156</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>-0.27363041899152879</c:v>
+                  <c:v>-0.27363040817363604</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>-0.27135037058589395</c:v>
+                  <c:v>-0.27135036283896757</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>-0.26967806466165845</c:v>
+                  <c:v>-0.26967805907043779</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>-0.26844952458160359</c:v>
+                  <c:v>-0.268449520522833</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>-0.26754592682403278</c:v>
+                  <c:v>-0.26754592386506326</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>-0.2668807520109866</c:v>
+                  <c:v>-0.26688074984697091</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>-0.26639077992376387</c:v>
+                  <c:v>-0.26639077833742736</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>-0.26602969546127081</c:v>
+                  <c:v>-0.26602969429639273</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>-0.26576350361143186</c:v>
+                  <c:v>-0.26576350275494681</c:v>
                 </c:pt>
                 <c:pt idx="31">
                   <c:v>0</c:v>
@@ -4596,7 +4594,7 @@
                   <c:v>5.7930026054258548</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>7.1946438481010171</c:v>
+                  <c:v>7.194643848101018</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>8.3581952718295298</c:v>
@@ -4605,79 +4603,79 @@
                   <c:v>9.3085326918379643</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>8.4662465705887264</c:v>
+                  <c:v>8.4662465705672627</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>6.4003136179165399</c:v>
+                  <c:v>6.4003136178987132</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>4.9210523377913526</c:v>
+                  <c:v>4.9210523377758104</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>4.7679254403556151</c:v>
+                  <c:v>4.767925440345735</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>4.8430504826626359</c:v>
+                  <c:v>4.8430504826584402</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>6.4021614369359519</c:v>
+                  <c:v>6.4021614369329081</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>7.7021400872290551</c:v>
+                  <c:v>7.7021400872267858</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>8.7748271560896463</c:v>
+                  <c:v>8.7748271560879694</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>9.6443153111210496</c:v>
+                  <c:v>9.6443151180901801</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>10.336527226893795</c:v>
+                  <c:v>10.336526968027982</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>10.878856438647293</c:v>
+                  <c:v>10.878856173459939</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>11.298090295969624</c:v>
+                  <c:v>11.29809005155264</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>11.618666049215198</c:v>
+                  <c:v>11.618665836176236</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>11.861706007590641</c:v>
+                  <c:v>11.861705828118161</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>12.044740115476579</c:v>
+                  <c:v>12.044739967655739</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>12.181882080925696</c:v>
+                  <c:v>12.181881961081082</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>12.284241393759546</c:v>
+                  <c:v>12.284241297704643</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>12.360417326524809</c:v>
+                  <c:v>12.360417250195674</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>12.416983807670961</c:v>
+                  <c:v>12.416983747415415</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>12.458920314836005</c:v>
+                  <c:v>12.458920267514916</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>12.489972937807559</c:v>
+                  <c:v>12.489972900798378</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>12.512945687615272</c:v>
+                  <c:v>12.512945658768956</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>12.529929593438927</c:v>
+                  <c:v>12.529929571018492</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>12.542479698678067</c:v>
+                  <c:v>12.542479681293722</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>12.551750094240138</c:v>
+                  <c:v>12.551750080788407</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -7510,16 +7508,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>451542</xdr:colOff>
-      <xdr:row>36</xdr:row>
-      <xdr:rowOff>155545</xdr:rowOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>478757</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>73902</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>98846</xdr:colOff>
-      <xdr:row>69</xdr:row>
-      <xdr:rowOff>179715</xdr:rowOff>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>112453</xdr:colOff>
+      <xdr:row>56</xdr:row>
+      <xdr:rowOff>98072</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -7965,36 +7963,35 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3BA97116-8F68-413B-968E-FF2BC2AA1259}">
   <dimension ref="A1:AE40"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="61" zoomScaleNormal="74" workbookViewId="0">
-      <selection activeCell="T6" sqref="T6"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="Y23" sqref="Y23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.06640625" customWidth="1"/>
-    <col min="2" max="2" width="4.796875" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="11.86328125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="20.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.19921875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.59765625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="18.46484375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.46484375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="5.53125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11.86328125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="14.33203125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="14.265625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="15.33203125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="14.59765625" customWidth="1"/>
-    <col min="16" max="16" width="16.6640625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="15.73046875" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="11.73046875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9" customWidth="1"/>
+    <col min="2" max="2" width="4.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="5.5703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="13" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="14.5703125" customWidth="1"/>
+    <col min="16" max="16" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="11.7109375" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="16" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="12.1328125" bestFit="1" customWidth="1"/>
-    <col min="21" max="22" width="12.46484375" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="11.86328125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="21" max="22" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="11.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:31" ht="18" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:31" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B1" t="s">
         <v>3</v>
       </c>
@@ -8023,7 +8020,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:31" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>4</v>
       </c>
@@ -8050,7 +8047,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="3" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
       <c r="B3" s="19" t="s">
         <v>0</v>
@@ -8096,7 +8093,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="4" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:31" x14ac:dyDescent="0.25">
       <c r="B4" s="7">
         <v>0</v>
       </c>
@@ -8137,11 +8134,11 @@
         <v>0.89905322734774096</v>
       </c>
       <c r="N4" s="15">
-        <f>-I4</f>
+        <f t="shared" ref="N4:N35" si="4">-I4</f>
         <v>-5.3623112246372617</v>
       </c>
       <c r="O4" s="13">
-        <f>E4*mass*K4</f>
+        <f t="shared" ref="O4:O35" si="5">E4*mass*K4</f>
         <v>0</v>
       </c>
       <c r="P4" s="21">
@@ -8149,7 +8146,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:31" x14ac:dyDescent="0.25">
       <c r="B5" s="7">
         <f>B4+0.5</f>
         <v>0.5</v>
@@ -8165,7 +8162,7 @@
         <v>3.3333333333333335</v>
       </c>
       <c r="F5" s="7">
-        <f t="shared" ref="F5:F35" si="4">D5+E5-0.02*K5^2</f>
+        <f t="shared" ref="F5:F35" si="6">D5+E5-0.02*K5^2</f>
         <v>6.2123865606810753</v>
       </c>
       <c r="G5" s="7"/>
@@ -8192,21 +8189,21 @@
         <v>3.3333334833333299</v>
       </c>
       <c r="N5" s="15">
-        <f>-I5</f>
+        <f t="shared" si="4"/>
         <v>-4.7510030086230293</v>
       </c>
       <c r="O5" s="13">
-        <f>E5*mass*K5</f>
+        <f t="shared" si="5"/>
         <v>500</v>
       </c>
       <c r="P5" s="21">
-        <f>IF(O5&gt;0,P4+O5*(B5-B4),P4)</f>
+        <f t="shared" ref="P5:P35" si="7">IF(O5&gt;0,P4+O5*(B5-B4),P4)</f>
         <v>250</v>
       </c>
     </row>
-    <row r="6" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:31" x14ac:dyDescent="0.25">
       <c r="B6" s="7">
-        <f t="shared" ref="B6:B35" si="5">B5+0.5</f>
+        <f t="shared" ref="B6:B35" si="8">B5+0.5</f>
         <v>1</v>
       </c>
       <c r="C6" s="7">
@@ -8220,7 +8217,7 @@
         <v>0.81178188793316886</v>
       </c>
       <c r="F6" s="7">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>3.3736186501706338</v>
       </c>
       <c r="G6" s="7"/>
@@ -8235,7 +8232,7 @@
         <v>1000</v>
       </c>
       <c r="K6" s="15">
-        <f t="shared" ref="K5:K35" si="6">F5*(B6-B5) + K5</f>
+        <f t="shared" ref="K6:K35" si="9">F5*(B6-B5) + K5</f>
         <v>4.1061932803405377</v>
       </c>
       <c r="L6" s="7">
@@ -8247,21 +8244,21 @@
         <v>0.81195696988029709</v>
       </c>
       <c r="N6" s="15">
-        <f>-I6</f>
+        <f t="shared" si="4"/>
         <v>-5.2430590466184501</v>
       </c>
       <c r="O6" s="13">
-        <f>E6*mass*K6</f>
+        <f t="shared" si="5"/>
         <v>500</v>
       </c>
       <c r="P6" s="21">
-        <f>IF(O6&gt;0,P5+O6*(B6-B5),P5)</f>
+        <f t="shared" si="7"/>
         <v>500</v>
       </c>
     </row>
-    <row r="7" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:31" x14ac:dyDescent="0.25">
       <c r="B7" s="7">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>1.5</v>
       </c>
       <c r="C7" s="7">
@@ -8272,11 +8269,11 @@
         <v>2.899053227347741</v>
       </c>
       <c r="E7" s="18">
-        <v>0.57540684173199907</v>
+        <v>0.57540684173199919</v>
       </c>
       <c r="F7" s="7">
-        <f t="shared" si="4"/>
-        <v>2.8032824853503251</v>
+        <f t="shared" si="6"/>
+        <v>2.8032824853503255</v>
       </c>
       <c r="G7" s="7"/>
       <c r="H7" s="7">
@@ -8290,7 +8287,7 @@
         <v>1000</v>
       </c>
       <c r="K7" s="15">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>5.7930026054258548</v>
       </c>
       <c r="L7" s="7">
@@ -8299,24 +8296,24 @@
       </c>
       <c r="M7" s="7">
         <f t="shared" si="3"/>
-        <v>0.57638462148486058</v>
+        <v>0.57638462148486069</v>
       </c>
       <c r="N7" s="15">
-        <f>-I7</f>
+        <f t="shared" si="4"/>
         <v>-4.8478537373624606</v>
       </c>
       <c r="O7" s="13">
-        <f>E7*mass*K7</f>
-        <v>499.99999999999994</v>
+        <f t="shared" si="5"/>
+        <v>500.00000000000006</v>
       </c>
       <c r="P7" s="21">
-        <f>IF(O7&gt;0,P6+O7*(B7-B6),P6)</f>
+        <f t="shared" si="7"/>
         <v>750</v>
       </c>
     </row>
-    <row r="8" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:31" x14ac:dyDescent="0.25">
       <c r="B8" s="7">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>2</v>
       </c>
       <c r="C8" s="7">
@@ -8327,10 +8324,10 @@
         <v>2.899053227347741</v>
       </c>
       <c r="E8" s="18">
-        <v>0.46330762212964111</v>
+        <v>0.46330762212964116</v>
       </c>
       <c r="F8" s="7">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>2.3271028474570254</v>
       </c>
       <c r="G8" s="7"/>
@@ -8345,33 +8342,33 @@
         <v>1000</v>
       </c>
       <c r="K8" s="15">
-        <f t="shared" si="6"/>
-        <v>7.1946438481010171</v>
+        <f t="shared" si="9"/>
+        <v>7.194643848101018</v>
       </c>
       <c r="L8" s="7">
         <f t="shared" si="2"/>
-        <v>5.1762900101017813E-2</v>
+        <v>5.1762900101017827E-2</v>
       </c>
       <c r="M8" s="7">
         <f t="shared" si="3"/>
-        <v>0.46619025145351362</v>
+        <v>0.46619025145351367</v>
       </c>
       <c r="N8" s="15">
-        <f>-I8</f>
+        <f t="shared" si="4"/>
         <v>-4.841227853590218</v>
       </c>
       <c r="O8" s="13">
-        <f>E8*mass*K8</f>
-        <v>499.99999999999994</v>
+        <f t="shared" si="5"/>
+        <v>500.00000000000011</v>
       </c>
       <c r="P8" s="21">
-        <f>IF(O8&gt;0,P7+O8*(B8-B7),P7)</f>
+        <f t="shared" si="7"/>
         <v>1000</v>
       </c>
     </row>
-    <row r="9" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:31" x14ac:dyDescent="0.25">
       <c r="B9" s="7">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>2.5</v>
       </c>
       <c r="C9" s="7">
@@ -8385,7 +8382,7 @@
         <v>0.39881017670979807</v>
       </c>
       <c r="F9" s="7">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>1.9006748400168687</v>
       </c>
       <c r="G9" s="7"/>
@@ -8393,14 +8390,14 @@
         <v>5.0992849719490048</v>
       </c>
       <c r="I9" s="15">
-        <f t="shared" ref="I9:I35" si="7">H9-0.3</f>
+        <f t="shared" ref="I9:I35" si="10">H9-0.3</f>
         <v>4.7992849719490049</v>
       </c>
       <c r="J9" s="16">
         <v>1000</v>
       </c>
       <c r="K9" s="15">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>8.3581952718295298</v>
       </c>
       <c r="L9" s="7">
@@ -8412,21 +8409,21 @@
         <v>0.4048825715636763</v>
       </c>
       <c r="N9" s="15">
-        <f>-I9</f>
+        <f t="shared" si="4"/>
         <v>-4.7992849719490049</v>
       </c>
       <c r="O9" s="13">
-        <f>E9*mass*K9</f>
+        <f t="shared" si="5"/>
         <v>500</v>
       </c>
       <c r="P9" s="21">
-        <f>IF(O9&gt;0,P8+O9*(B9-B8),P8)</f>
+        <f t="shared" si="7"/>
         <v>1250</v>
       </c>
     </row>
-    <row r="10" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:31" x14ac:dyDescent="0.25">
       <c r="B10" s="7">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>3</v>
       </c>
       <c r="C10" s="7">
@@ -8437,25 +8434,25 @@
         <v>2.899053227347741</v>
       </c>
       <c r="E10" s="18">
-        <v>-2.8506498523458927</v>
+        <v>-2.8506498523888202</v>
       </c>
       <c r="F10" s="7">
-        <f t="shared" si="4"/>
-        <v>-1.6845722424984746</v>
+        <f t="shared" si="6"/>
+        <v>-1.684572242541402</v>
       </c>
       <c r="G10" s="7"/>
       <c r="H10" s="7">
         <v>5.2673372817725035</v>
       </c>
       <c r="I10" s="15">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>4.9673372817725037</v>
       </c>
       <c r="J10" s="16">
         <v>1000</v>
       </c>
       <c r="K10" s="15">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>9.3085326918379643</v>
       </c>
       <c r="L10" s="7">
@@ -8464,24 +8461,24 @@
       </c>
       <c r="M10" s="7">
         <f t="shared" si="3"/>
-        <v>2.8519664429839962</v>
+        <v>2.8519664430269036</v>
       </c>
       <c r="N10" s="15">
-        <f>-I10</f>
+        <f t="shared" si="4"/>
         <v>-4.9673372817725037</v>
       </c>
       <c r="O10" s="13">
-        <f>E10*mass*K10</f>
-        <v>-3980.3051015317214</v>
+        <f t="shared" si="5"/>
+        <v>-3980.3051015916599</v>
       </c>
       <c r="P10" s="21">
-        <f>IF(O10&gt;0,P9+O10*(B10-B9),P9)</f>
+        <f t="shared" si="7"/>
         <v>1250</v>
       </c>
     </row>
-    <row r="11" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:31" x14ac:dyDescent="0.25">
       <c r="B11" s="7">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>3.5</v>
       </c>
       <c r="C11" s="7">
@@ -8492,51 +8489,51 @@
         <v>2.899053227347741</v>
       </c>
       <c r="E11" s="18">
-        <v>-5.5973725128120062</v>
+        <v>-5.5973725128120009</v>
       </c>
       <c r="F11" s="7">
-        <f t="shared" si="4"/>
-        <v>-4.1318659053443731</v>
+        <f t="shared" si="6"/>
+        <v>-4.131865905337099</v>
       </c>
       <c r="G11" s="7"/>
       <c r="H11" s="7">
         <v>5.8978314271655066</v>
       </c>
       <c r="I11" s="15">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>5.5978314271655067</v>
       </c>
       <c r="J11" s="16">
         <v>1000</v>
       </c>
       <c r="K11" s="15">
-        <f t="shared" si="6"/>
-        <v>8.4662465705887264</v>
+        <f t="shared" si="9"/>
+        <v>8.4662465705672627</v>
       </c>
       <c r="L11" s="7">
         <f t="shared" si="2"/>
-        <v>7.1677330994005375E-2</v>
+        <v>7.167733099364193E-2</v>
       </c>
       <c r="M11" s="7">
         <f t="shared" si="3"/>
-        <v>5.5978314271655067</v>
+        <v>5.597831427165497</v>
       </c>
       <c r="N11" s="15">
-        <f>-I11</f>
+        <f t="shared" si="4"/>
         <v>-5.5978314271655067</v>
       </c>
       <c r="O11" s="13">
-        <f>E11*mass*K11</f>
-        <v>-7108.3103761353377</v>
+        <f t="shared" si="5"/>
+        <v>-7108.3103761173097</v>
       </c>
       <c r="P11" s="21">
-        <f>IF(O11&gt;0,P10+O11*(B11-B10),P10)</f>
+        <f t="shared" si="7"/>
         <v>1250</v>
       </c>
     </row>
-    <row r="12" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:31" x14ac:dyDescent="0.25">
       <c r="B12" s="7">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>4</v>
       </c>
       <c r="C12" s="7">
@@ -8547,51 +8544,51 @@
         <v>2.899053227347741</v>
       </c>
       <c r="E12" s="18">
-        <v>-5.0382954994443567</v>
+        <v>-5.0382954994443523</v>
       </c>
       <c r="F12" s="7">
-        <f t="shared" si="4"/>
-        <v>-2.958522560250374</v>
+        <f t="shared" si="6"/>
+        <v>-2.9585225602458056</v>
       </c>
       <c r="G12" s="7"/>
       <c r="H12" s="7">
         <v>5.3384620262732607</v>
       </c>
       <c r="I12" s="15">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>5.0384620262732609</v>
       </c>
       <c r="J12" s="16">
         <v>1000</v>
       </c>
       <c r="K12" s="15">
-        <f t="shared" si="6"/>
-        <v>6.4003136179165399</v>
+        <f t="shared" si="9"/>
+        <v>6.4003136178987132</v>
       </c>
       <c r="L12" s="7">
         <f t="shared" si="2"/>
-        <v>4.0964014407687904E-2</v>
+        <v>4.0964014407459712E-2</v>
       </c>
       <c r="M12" s="7">
         <f t="shared" si="3"/>
-        <v>5.0384620262732609</v>
+        <v>5.0384620262732547</v>
       </c>
       <c r="N12" s="15">
-        <f>-I12</f>
+        <f t="shared" si="4"/>
         <v>-5.0384620262732609</v>
       </c>
       <c r="O12" s="13">
-        <f>E12*mass*K12</f>
-        <v>-4837.0006944271991</v>
+        <f t="shared" si="5"/>
+        <v>-4837.0006944137231</v>
       </c>
       <c r="P12" s="21">
-        <f>IF(O12&gt;0,P11+O12*(B12-B11),P11)</f>
+        <f t="shared" si="7"/>
         <v>1250</v>
       </c>
     </row>
-    <row r="13" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:31" x14ac:dyDescent="0.25">
       <c r="B13" s="7">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>4.5</v>
       </c>
       <c r="C13" s="7">
@@ -8602,51 +8599,51 @@
         <v>2.899053227347741</v>
       </c>
       <c r="E13" s="18">
-        <v>-2.720971899993581</v>
+        <v>-2.7209718999853165</v>
       </c>
       <c r="F13" s="7">
-        <f t="shared" si="4"/>
-        <v>-0.3062537948714748</v>
+        <f t="shared" si="6"/>
+        <v>-0.30625379486015097</v>
       </c>
       <c r="G13" s="7"/>
       <c r="H13" s="7">
         <v>5.8553342962135719</v>
       </c>
       <c r="I13" s="15">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>5.5553342962135721</v>
       </c>
       <c r="J13" s="16">
         <v>5</v>
       </c>
       <c r="K13" s="15">
-        <f t="shared" si="6"/>
-        <v>4.9210523377913526</v>
+        <f t="shared" si="9"/>
+        <v>4.9210523377758104</v>
       </c>
       <c r="L13" s="7">
-        <f t="shared" ref="L13:L27" si="8">K13^2/J13</f>
-        <v>4.8433512222563468</v>
+        <f t="shared" ref="L13:L27" si="11">K13^2/J13</f>
+        <v>4.8433512222257544</v>
       </c>
       <c r="M13" s="7">
         <f t="shared" si="3"/>
-        <v>5.5553342962135712</v>
+        <v>5.5553342961828509</v>
       </c>
       <c r="N13" s="15">
-        <f>-I13</f>
+        <f t="shared" si="4"/>
         <v>-5.5553342962135721</v>
       </c>
       <c r="O13" s="13">
-        <f>E13*mass*K13</f>
-        <v>-2008.5067694291986</v>
+        <f t="shared" si="5"/>
+        <v>-2008.5067694167547</v>
       </c>
       <c r="P13" s="21">
-        <f>IF(O13&gt;0,P12+O13*(B13-B12),P12)</f>
+        <f t="shared" si="7"/>
         <v>1250</v>
       </c>
     </row>
-    <row r="14" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:31" x14ac:dyDescent="0.25">
       <c r="B14" s="7">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>5</v>
       </c>
       <c r="C14" s="7">
@@ -8657,51 +8654,51 @@
         <v>2.899053227347741</v>
       </c>
       <c r="E14" s="18">
-        <v>-2.294140882637894</v>
+        <v>-2.2941408826284087</v>
       </c>
       <c r="F14" s="7">
-        <f t="shared" si="4"/>
-        <v>0.15025008461404127</v>
+        <f t="shared" si="6"/>
+        <v>0.15025008462541084</v>
       </c>
       <c r="G14" s="7"/>
       <c r="H14" s="7">
         <v>5.3926279527306145</v>
       </c>
       <c r="I14" s="15">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>5.0926279527306146</v>
       </c>
       <c r="J14" s="16">
         <v>5</v>
       </c>
       <c r="K14" s="15">
-        <f t="shared" si="6"/>
-        <v>4.7679254403556151</v>
+        <f t="shared" si="9"/>
+        <v>4.767925440345735</v>
       </c>
       <c r="L14" s="7">
-        <f t="shared" si="8"/>
-        <v>4.5466226009580577</v>
+        <f t="shared" si="11"/>
+        <v>4.5466226009392141</v>
       </c>
       <c r="M14" s="7">
         <f t="shared" si="3"/>
-        <v>5.0926279527306129</v>
+        <v>5.092627952709516</v>
       </c>
       <c r="N14" s="15">
-        <f>-I14</f>
+        <f t="shared" si="4"/>
         <v>-5.0926279527306146</v>
       </c>
       <c r="O14" s="13">
-        <f>E14*mass*K14</f>
-        <v>-1640.7439017133649</v>
+        <f t="shared" si="5"/>
+        <v>-1640.7439017031811</v>
       </c>
       <c r="P14" s="21">
-        <f>IF(O14&gt;0,P13+O14*(B14-B13),P13)</f>
+        <f t="shared" si="7"/>
         <v>1250</v>
       </c>
     </row>
-    <row r="15" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:31" x14ac:dyDescent="0.25">
       <c r="B15" s="7">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>5.5</v>
       </c>
       <c r="C15" s="7">
@@ -8712,51 +8709,51 @@
         <v>2.899053227347741</v>
       </c>
       <c r="E15" s="18">
-        <v>0.68827144075126734</v>
+        <v>0.68827144075275781</v>
       </c>
       <c r="F15" s="7">
-        <f t="shared" si="4"/>
-        <v>3.1182219085466327</v>
+        <f t="shared" si="6"/>
+        <v>3.1182219085489358</v>
       </c>
       <c r="G15" s="7"/>
       <c r="H15" s="7">
         <v>5.0412506238459125</v>
       </c>
       <c r="I15" s="15">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>4.7412506238459127</v>
       </c>
       <c r="J15" s="16">
         <v>5</v>
       </c>
       <c r="K15" s="15">
-        <f t="shared" si="6"/>
-        <v>4.8430504826626359</v>
+        <f t="shared" si="9"/>
+        <v>4.8430504826584402</v>
       </c>
       <c r="L15" s="7">
-        <f t="shared" si="8"/>
-        <v>4.6910275955237584</v>
+        <f t="shared" si="11"/>
+        <v>4.6910275955156298</v>
       </c>
       <c r="M15" s="7">
         <f t="shared" si="3"/>
-        <v>4.7412506238459109</v>
+        <v>4.7412506238380852</v>
       </c>
       <c r="N15" s="15">
-        <f>-I15</f>
+        <f t="shared" si="4"/>
         <v>-4.7412506238459127</v>
       </c>
       <c r="O15" s="13">
-        <f>E15*mass*K15</f>
-        <v>499.99999999999994</v>
+        <f t="shared" si="5"/>
+        <v>500.00000000064955</v>
       </c>
       <c r="P15" s="21">
-        <f>IF(O15&gt;0,P14+O15*(B15-B14),P14)</f>
-        <v>1500</v>
+        <f t="shared" si="7"/>
+        <v>1500.0000000003247</v>
       </c>
     </row>
-    <row r="16" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:31" x14ac:dyDescent="0.25">
       <c r="B16" s="7">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>6</v>
       </c>
       <c r="C16" s="7">
@@ -8767,51 +8764,51 @@
         <v>2.899053227347741</v>
       </c>
       <c r="E16" s="18">
-        <v>0.52065749453026178</v>
+        <v>0.52065749453103116</v>
       </c>
       <c r="F16" s="7">
-        <f t="shared" si="4"/>
-        <v>2.5999573005862064</v>
+        <f t="shared" si="6"/>
+        <v>2.5999573005877554</v>
       </c>
       <c r="G16" s="7"/>
       <c r="H16" s="7">
         <v>5.716598475865827</v>
       </c>
       <c r="I16" s="15">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>5.4165984758658272</v>
       </c>
       <c r="J16" s="16">
         <v>1000</v>
       </c>
       <c r="K16" s="15">
-        <f t="shared" si="6"/>
-        <v>6.4021614369359519</v>
+        <f t="shared" si="9"/>
+        <v>6.4021614369329081</v>
       </c>
       <c r="L16" s="7">
-        <f t="shared" si="8"/>
-        <v>4.0987671064589809E-2</v>
+        <f t="shared" si="11"/>
+        <v>4.098767106455084E-2</v>
       </c>
       <c r="M16" s="7">
         <f t="shared" si="3"/>
-        <v>0.52226833695891284</v>
+        <v>0.52226833695967678</v>
       </c>
       <c r="N16" s="15">
-        <f>-I16</f>
+        <f t="shared" si="4"/>
         <v>-5.4165984758658272</v>
       </c>
       <c r="O16" s="13">
-        <f>E16*mass*K16</f>
-        <v>500</v>
+        <f t="shared" si="5"/>
+        <v>500.00000000050113</v>
       </c>
       <c r="P16" s="21">
-        <f>IF(O16&gt;0,P15+O16*(B16-B15),P15)</f>
-        <v>1750</v>
+        <f t="shared" si="7"/>
+        <v>1750.0000000005753</v>
       </c>
     </row>
-    <row r="17" spans="2:19" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="17" spans="2:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B17" s="7">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>6.5</v>
       </c>
       <c r="C17" s="7">
@@ -8822,51 +8819,51 @@
         <v>2.899053227347741</v>
       </c>
       <c r="E17" s="18">
-        <v>0.43278014883945631</v>
+        <v>0.43278014883994498</v>
       </c>
       <c r="F17" s="7">
-        <f t="shared" si="4"/>
-        <v>2.1453741377211815</v>
+        <f t="shared" si="6"/>
+        <v>2.145374137722369</v>
       </c>
       <c r="G17" s="7"/>
       <c r="H17" s="7">
         <v>5.6642566000684162</v>
       </c>
       <c r="I17" s="15">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>5.3642566000684164</v>
       </c>
       <c r="J17" s="16">
         <v>1000</v>
       </c>
       <c r="K17" s="15">
-        <f t="shared" si="6"/>
-        <v>7.7021400872290551</v>
+        <f t="shared" si="9"/>
+        <v>7.7021400872267858</v>
       </c>
       <c r="L17" s="7">
-        <f t="shared" si="8"/>
-        <v>5.9322961923300797E-2</v>
+        <f t="shared" si="11"/>
+        <v>5.9322961923265839E-2</v>
       </c>
       <c r="M17" s="7">
         <f t="shared" si="3"/>
-        <v>0.43682704934659822</v>
+        <v>0.43682704934707761</v>
       </c>
       <c r="N17" s="15">
-        <f>-I17</f>
+        <f t="shared" si="4"/>
         <v>-5.3642566000684164</v>
       </c>
       <c r="O17" s="13">
-        <f>E17*mass*K17</f>
-        <v>500.00000000000006</v>
+        <f t="shared" si="5"/>
+        <v>500.00000000041729</v>
       </c>
       <c r="P17" s="21">
-        <f>IF(O17&gt;0,P16+O17*(B17-B16),P16)</f>
-        <v>2000</v>
+        <f t="shared" si="7"/>
+        <v>2000.000000000784</v>
       </c>
     </row>
-    <row r="18" spans="2:19" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="18" spans="2:19" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B18" s="7">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>7</v>
       </c>
       <c r="C18" s="7">
@@ -8877,54 +8874,54 @@
         <v>2.899053227347741</v>
       </c>
       <c r="E18" s="18">
-        <v>0.37987491510003324</v>
+        <v>0.37987452904105873</v>
       </c>
       <c r="F18" s="7">
-        <f t="shared" si="4"/>
-        <v>1.7389763100628077</v>
+        <f t="shared" si="6"/>
+        <v>1.7389759240044218</v>
       </c>
       <c r="G18" s="7"/>
       <c r="H18" s="7">
         <v>5.2013230540525672</v>
       </c>
       <c r="I18" s="15">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>4.9013230540525674</v>
       </c>
       <c r="J18" s="16">
         <v>1000</v>
       </c>
       <c r="K18" s="15">
-        <f t="shared" si="6"/>
-        <v>8.7748271560896463</v>
+        <f t="shared" si="9"/>
+        <v>8.7748271560879694</v>
       </c>
       <c r="L18" s="7">
-        <f t="shared" si="8"/>
-        <v>7.699759161924831E-2</v>
+        <f t="shared" si="11"/>
+        <v>7.6997591619218875E-2</v>
       </c>
       <c r="M18" s="7">
         <f t="shared" si="3"/>
-        <v>0.38759976810806013</v>
+        <v>0.38759938974323244</v>
       </c>
       <c r="N18" s="15">
-        <f>-I18</f>
+        <f t="shared" si="4"/>
         <v>-4.9013230540525674</v>
       </c>
       <c r="O18" s="13">
-        <f>E18*mass*K18</f>
-        <v>500.00050814055305</v>
+        <f t="shared" si="5"/>
+        <v>500.00000000034152</v>
       </c>
       <c r="P18" s="21">
-        <f>IF(O18&gt;0,P17+O18*(B18-B17),P17)</f>
-        <v>2250.0002540702767</v>
+        <f t="shared" si="7"/>
+        <v>2250.000000000955</v>
       </c>
       <c r="S18" s="14" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="19" spans="2:19" x14ac:dyDescent="0.45">
+    <row r="19" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B19" s="7">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>7.5</v>
       </c>
       <c r="C19" s="7">
@@ -8935,54 +8932,54 @@
         <v>2.899053227347741</v>
       </c>
       <c r="E19" s="18">
-        <v>0.3456269606042266</v>
+        <v>0.3456267544683212</v>
       </c>
       <c r="F19" s="7">
-        <f t="shared" si="4"/>
-        <v>1.3844238315454895</v>
+        <f t="shared" si="6"/>
+        <v>1.3844236998756063</v>
       </c>
       <c r="G19" s="7"/>
       <c r="H19" s="7">
         <v>5.5945634273547507</v>
       </c>
       <c r="I19" s="15">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>5.2945634273547508</v>
       </c>
       <c r="J19" s="16">
         <v>1000</v>
       </c>
       <c r="K19" s="15">
-        <f t="shared" si="6"/>
-        <v>9.6443153111210496</v>
+        <f t="shared" si="9"/>
+        <v>9.6443151180901801</v>
       </c>
       <c r="L19" s="7">
-        <f t="shared" si="8"/>
-        <v>9.3012817820323904E-2</v>
+        <f t="shared" si="11"/>
+        <v>9.3012814097022792E-2</v>
       </c>
       <c r="M19" s="7">
         <f t="shared" si="3"/>
-        <v>0.35792370719944266</v>
+        <v>0.35792350717793392</v>
       </c>
       <c r="N19" s="15">
-        <f>-I19</f>
+        <f t="shared" si="4"/>
         <v>-5.2945634273547508</v>
       </c>
       <c r="O19" s="13">
-        <f>E19*mass*K19</f>
-        <v>500.0003082137361</v>
+        <f t="shared" si="5"/>
+        <v>500.00000000029092</v>
       </c>
       <c r="P19" s="21">
-        <f>IF(O19&gt;0,P18+O19*(B19-B18),P18)</f>
-        <v>2500.0004081771449</v>
+        <f t="shared" si="7"/>
+        <v>2500.0000000011005</v>
       </c>
       <c r="S19" s="2" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="20" spans="2:19" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="20" spans="2:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B20" s="7">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>8</v>
       </c>
       <c r="C20" s="7">
@@ -8993,55 +8990,55 @@
         <v>2.899053227347741</v>
       </c>
       <c r="E20" s="18">
-        <v>0.32248109840558953</v>
+        <v>0.32248097873156589</v>
       </c>
       <c r="F20" s="7">
-        <f t="shared" si="4"/>
-        <v>1.0846584235069963</v>
+        <f t="shared" si="6"/>
+        <v>1.0846584108639115</v>
       </c>
       <c r="G20" s="7"/>
       <c r="H20" s="7">
         <v>5.0084589497584355</v>
       </c>
       <c r="I20" s="15">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>4.7084589497584357</v>
       </c>
       <c r="J20" s="16">
         <v>1000</v>
       </c>
       <c r="K20" s="15">
-        <f t="shared" si="6"/>
-        <v>10.336527226893795</v>
+        <f t="shared" si="9"/>
+        <v>10.336526968027982</v>
       </c>
       <c r="L20" s="7">
-        <f t="shared" si="8"/>
-        <v>0.10684379511231673</v>
+        <f t="shared" si="11"/>
+        <v>0.10684378976076975</v>
       </c>
       <c r="M20" s="7">
         <f t="shared" si="3"/>
-        <v>0.33971996612339145</v>
+        <v>0.33971985083905859</v>
       </c>
       <c r="N20" s="15">
-        <f>-I20</f>
+        <f t="shared" si="4"/>
         <v>-4.7084589497584357</v>
       </c>
       <c r="O20" s="13">
-        <f>E20*mass*K20</f>
-        <v>500.00019807419898</v>
+        <f t="shared" si="5"/>
+        <v>500.0000000002334</v>
       </c>
       <c r="P20" s="21">
-        <f>IF(O20&gt;0,P19+O20*(B20-B19),P19)</f>
-        <v>2750.0005072142444</v>
+        <f t="shared" si="7"/>
+        <v>2750.0000000012174</v>
       </c>
       <c r="S20" s="17">
         <f>AVERAGE(K4:K35)*B35</f>
-        <v>140.49331227239034</v>
+        <v>140.49331129355255</v>
       </c>
     </row>
-    <row r="21" spans="2:19" x14ac:dyDescent="0.45">
+    <row r="21" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B21" s="7">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>8.5</v>
       </c>
       <c r="C21" s="7">
@@ -9052,51 +9049,51 @@
         <v>2.899053227347741</v>
       </c>
       <c r="E21" s="18">
-        <v>0.30640483555087467</v>
+        <v>0.30640476169421088</v>
       </c>
       <c r="F21" s="7">
         <f>D21+E21-0.02*K21^2</f>
-        <v>0.83846771464466219</v>
+        <v>0.83846775618540326</v>
       </c>
       <c r="G21" s="7"/>
       <c r="H21" s="7">
         <v>5.9037745401277535</v>
       </c>
       <c r="I21" s="15">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>5.6037745401277537</v>
       </c>
       <c r="J21" s="16">
         <v>1000</v>
       </c>
       <c r="K21" s="15">
-        <f t="shared" si="6"/>
-        <v>10.878856438647293</v>
+        <f t="shared" si="9"/>
+        <v>10.878856173459939</v>
       </c>
       <c r="L21" s="7">
-        <f t="shared" si="8"/>
-        <v>0.11834951741269768</v>
+        <f t="shared" si="11"/>
+        <v>0.11834951164282742</v>
       </c>
       <c r="M21" s="7">
         <f>SQRT((L21)^2+E21^2)</f>
-        <v>0.3284669412905612</v>
+        <v>0.32846687031568633</v>
       </c>
       <c r="N21" s="15">
-        <f>-I21</f>
+        <f t="shared" si="4"/>
         <v>-5.6037745401277537</v>
       </c>
       <c r="O21" s="13">
-        <f>E21*mass*K21</f>
-        <v>500.00013270979468</v>
+        <f t="shared" si="5"/>
+        <v>500.00000000018809</v>
       </c>
       <c r="P21" s="21">
-        <f>IF(O21&gt;0,P20+O21*(B21-B20),P20)</f>
-        <v>3000.0005735691416</v>
+        <f t="shared" si="7"/>
+        <v>3000.0000000013115</v>
       </c>
     </row>
-    <row r="22" spans="2:19" x14ac:dyDescent="0.45">
+    <row r="22" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B22" s="7">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>9</v>
       </c>
       <c r="C22" s="7">
@@ -9107,51 +9104,51 @@
         <v>2.899053227347741</v>
       </c>
       <c r="E22" s="18">
-        <v>0.2950351658610682</v>
+        <v>0.29503511815930472</v>
       </c>
       <c r="F22" s="7">
         <f>D22+E22-0.02*K22^2</f>
-        <v>0.64115150649114971</v>
+        <v>0.64115156924719141</v>
       </c>
       <c r="G22" s="7"/>
       <c r="H22" s="7">
         <v>5.9019712484700415</v>
       </c>
       <c r="I22" s="15">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>5.6019712484700417</v>
       </c>
       <c r="J22" s="16">
         <v>1000</v>
       </c>
       <c r="K22" s="15">
-        <f t="shared" si="6"/>
-        <v>11.298090295969624</v>
+        <f t="shared" si="9"/>
+        <v>11.29809005155264</v>
       </c>
       <c r="L22" s="7">
-        <f t="shared" si="8"/>
-        <v>0.127646844335883</v>
+        <f t="shared" si="11"/>
+        <v>0.12764683881299271</v>
       </c>
       <c r="M22" s="7">
         <f t="shared" si="3"/>
-        <v>0.32146456408689461</v>
+        <v>0.32146451811393595</v>
       </c>
       <c r="N22" s="15">
-        <f>-I22</f>
+        <f t="shared" si="4"/>
         <v>-5.6019712484700417</v>
       </c>
       <c r="O22" s="13">
-        <f>E22*mass*K22</f>
-        <v>500.00009165770848</v>
+        <f t="shared" si="5"/>
+        <v>500.00000000014472</v>
       </c>
       <c r="P22" s="21">
-        <f>IF(O22&gt;0,P21+O22*(B22-B21),P21)</f>
-        <v>3250.0006193979957</v>
+        <f t="shared" si="7"/>
+        <v>3250.0000000013838</v>
       </c>
     </row>
-    <row r="23" spans="2:19" x14ac:dyDescent="0.45">
+    <row r="23" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B23" s="7">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>9.5</v>
       </c>
       <c r="C23" s="7">
@@ -9162,18 +9159,18 @@
         <v>2.899053227347741</v>
       </c>
       <c r="E23" s="18">
-        <v>0.2868947046668639</v>
+        <v>0.2868946727906857</v>
       </c>
       <c r="F23" s="7">
-        <f t="shared" si="4"/>
-        <v>0.48607991675088646</v>
+        <f t="shared" si="6"/>
+        <v>0.48607998388384965</v>
       </c>
       <c r="G23" s="7"/>
       <c r="H23" s="7">
         <v>5.858501477726394</v>
       </c>
       <c r="I23" s="15">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>5.5585014777263941</v>
       </c>
       <c r="J23" s="16">
@@ -9181,32 +9178,32 @@
       </c>
       <c r="K23" s="15">
         <f>F22*(B23-B22) + K22</f>
-        <v>11.618666049215198</v>
+        <v>11.618665836176236</v>
       </c>
       <c r="L23" s="7">
-        <f t="shared" si="8"/>
-        <v>0.13499340076318592</v>
+        <f t="shared" si="11"/>
+        <v>0.13499339581272884</v>
       </c>
       <c r="M23" s="7">
         <f t="shared" si="3"/>
-        <v>0.31706748463930701</v>
+        <v>0.31706745368884315</v>
       </c>
       <c r="N23" s="15">
-        <f>-I23</f>
+        <f t="shared" si="4"/>
         <v>-5.5585014777263941</v>
       </c>
       <c r="O23" s="13">
-        <f>E23*mass*K23</f>
-        <v>500.00006472187692</v>
+        <f t="shared" si="5"/>
+        <v>500.00000000011499</v>
       </c>
       <c r="P23" s="21">
-        <f>IF(O23&gt;0,P22+O23*(B23-B22),P22)</f>
-        <v>3500.0006517589341</v>
+        <f t="shared" si="7"/>
+        <v>3500.0000000014411</v>
       </c>
     </row>
-    <row r="24" spans="2:19" x14ac:dyDescent="0.45">
+    <row r="24" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B24" s="7">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>10</v>
       </c>
       <c r="C24" s="7">
@@ -9217,51 +9214,51 @@
         <v>2.899053227347741</v>
       </c>
       <c r="E24" s="18">
-        <v>0.28101637663437412</v>
+        <v>0.28101635478366221</v>
       </c>
       <c r="F24" s="7">
-        <f t="shared" si="4"/>
-        <v>0.36606821577187709</v>
+        <f t="shared" si="6"/>
+        <v>0.36606827907515571</v>
       </c>
       <c r="G24" s="7"/>
       <c r="H24" s="7">
         <v>5.772152436561262</v>
       </c>
       <c r="I24" s="15">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>5.4721524365612622</v>
       </c>
       <c r="J24" s="16">
         <v>1000</v>
       </c>
       <c r="K24" s="15">
-        <f t="shared" si="6"/>
-        <v>11.861706007590641</v>
+        <f t="shared" si="9"/>
+        <v>11.861705828118161</v>
       </c>
       <c r="L24" s="7">
-        <f t="shared" si="8"/>
-        <v>0.14070006941051191</v>
+        <f t="shared" si="11"/>
+        <v>0.14070006515281236</v>
       </c>
       <c r="M24" s="7">
         <f t="shared" si="3"/>
-        <v>0.31427171916803981</v>
+        <v>0.31427169772332786</v>
       </c>
       <c r="N24" s="15">
-        <f>-I24</f>
+        <f t="shared" si="4"/>
         <v>-5.4721524365612622</v>
       </c>
       <c r="O24" s="13">
-        <f>E24*mass*K24</f>
-        <v>500.00004644329641</v>
+        <f t="shared" si="5"/>
+        <v>500.00000000008299</v>
       </c>
       <c r="P24" s="21">
-        <f>IF(O24&gt;0,P23+O24*(B24-B23),P23)</f>
-        <v>3750.0006749805821</v>
+        <f t="shared" si="7"/>
+        <v>3750.0000000014825</v>
       </c>
     </row>
-    <row r="25" spans="2:19" x14ac:dyDescent="0.45">
+    <row r="25" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B25" s="7">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>10.5</v>
       </c>
       <c r="C25" s="7">
@@ -9272,51 +9269,51 @@
         <v>2.899053227347741</v>
       </c>
       <c r="E25" s="18">
-        <v>0.27674599253790766</v>
+        <v>0.2767459772718156</v>
       </c>
       <c r="F25" s="7">
-        <f t="shared" si="4"/>
-        <v>0.27428393089823366</v>
+        <f t="shared" si="6"/>
+        <v>0.27428398685068522</v>
       </c>
       <c r="G25" s="7"/>
       <c r="H25" s="7">
         <v>5.5098794438847687</v>
       </c>
       <c r="I25" s="15">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>5.2098794438847689</v>
       </c>
       <c r="J25" s="16">
         <v>1000</v>
       </c>
       <c r="K25" s="15">
-        <f t="shared" si="6"/>
-        <v>12.044740115476579</v>
+        <f t="shared" si="9"/>
+        <v>12.044739967655739</v>
       </c>
       <c r="L25" s="7">
-        <f t="shared" si="8"/>
-        <v>0.14507576444937076</v>
+        <f t="shared" si="11"/>
+        <v>0.14507576088844357</v>
       </c>
       <c r="M25" s="7">
         <f t="shared" si="3"/>
-        <v>0.31246651311198287</v>
+        <v>0.31246649793776793</v>
       </c>
       <c r="N25" s="15">
-        <f>-I25</f>
+        <f t="shared" si="4"/>
         <v>-5.2098794438847689</v>
       </c>
       <c r="O25" s="13">
-        <f>E25*mass*K25</f>
-        <v>500.0000337178077</v>
+        <f t="shared" si="5"/>
+        <v>500.00000000006759</v>
       </c>
       <c r="P25" s="21">
-        <f>IF(O25&gt;0,P24+O25*(B25-B24),P24)</f>
-        <v>4000.0006918394861</v>
+        <f t="shared" si="7"/>
+        <v>4000.0000000015161</v>
       </c>
     </row>
-    <row r="26" spans="2:19" x14ac:dyDescent="0.45">
+    <row r="26" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B26" s="7">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>11</v>
       </c>
       <c r="C26" s="7">
@@ -9327,51 +9324,51 @@
         <v>2.899053227347741</v>
       </c>
       <c r="E26" s="18">
-        <v>0.27363041899152879</v>
+        <v>0.27363040817363604</v>
       </c>
       <c r="F26" s="7">
-        <f t="shared" si="4"/>
-        <v>0.20471862566769872</v>
+        <f t="shared" si="6"/>
+        <v>0.20471867324712356</v>
       </c>
       <c r="G26" s="7"/>
       <c r="H26" s="7">
         <v>5.39413195880892</v>
       </c>
       <c r="I26" s="15">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>5.0941319588089202</v>
       </c>
       <c r="J26" s="16">
         <v>1000</v>
       </c>
       <c r="K26" s="15">
-        <f t="shared" si="6"/>
-        <v>12.181882080925696</v>
+        <f t="shared" si="9"/>
+        <v>12.181881961081082</v>
       </c>
       <c r="L26" s="7">
-        <f t="shared" si="8"/>
-        <v>0.14839825103357857</v>
+        <f t="shared" si="11"/>
+        <v>0.14839824811371266</v>
       </c>
       <c r="M26" s="7">
         <f t="shared" si="3"/>
-        <v>0.31128065649395015</v>
+        <v>0.31128064559250979</v>
       </c>
       <c r="N26" s="15">
-        <f>-I26</f>
+        <f t="shared" si="4"/>
         <v>-5.0941319588089202</v>
       </c>
       <c r="O26" s="13">
-        <f>E26*mass*K26</f>
-        <v>500.00002468636427</v>
+        <f t="shared" si="5"/>
+        <v>500.00000000005053</v>
       </c>
       <c r="P26" s="21">
-        <f>IF(O26&gt;0,P25+O26*(B26-B25),P25)</f>
-        <v>4250.0007041826684</v>
+        <f t="shared" si="7"/>
+        <v>4250.0000000015416</v>
       </c>
     </row>
-    <row r="27" spans="2:19" x14ac:dyDescent="0.45">
+    <row r="27" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B27" s="7">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>11.5</v>
       </c>
       <c r="C27" s="7">
@@ -9382,51 +9379,51 @@
         <v>2.899053227347741</v>
       </c>
       <c r="E27" s="18">
-        <v>0.27135037058589395</v>
+        <v>0.27135036283896757</v>
       </c>
       <c r="F27" s="7">
-        <f t="shared" si="4"/>
-        <v>0.15235186553052582</v>
+        <f t="shared" si="6"/>
+        <v>0.15235190498206341</v>
       </c>
       <c r="G27" s="7"/>
       <c r="H27" s="7">
         <v>5.6548419761332624</v>
       </c>
       <c r="I27" s="15">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>5.3548419761332626</v>
       </c>
       <c r="J27" s="16">
         <v>1000</v>
       </c>
       <c r="K27" s="15">
-        <f t="shared" si="6"/>
-        <v>12.284241393759546</v>
+        <f t="shared" si="9"/>
+        <v>12.284241297704643</v>
       </c>
       <c r="L27" s="7">
-        <f t="shared" si="8"/>
-        <v>0.15090258662015546</v>
+        <f t="shared" si="11"/>
+        <v>0.15090258426023226</v>
       </c>
       <c r="M27" s="7">
         <f t="shared" si="3"/>
-        <v>0.3104877038881822</v>
+        <v>0.31048769597079984</v>
       </c>
       <c r="N27" s="15">
-        <f>-I27</f>
+        <f t="shared" si="4"/>
         <v>-5.3548419761332626</v>
       </c>
       <c r="O27" s="13">
-        <f>E27*mass*K27</f>
-        <v>500.00001818448465</v>
+        <f t="shared" si="5"/>
+        <v>500.00000000003769</v>
       </c>
       <c r="P27" s="21">
-        <f>IF(O27&gt;0,P26+O27*(B27-B26),P26)</f>
-        <v>4500.0007132749106</v>
+        <f t="shared" si="7"/>
+        <v>4500.0000000015607</v>
       </c>
     </row>
-    <row r="28" spans="2:19" x14ac:dyDescent="0.45">
+    <row r="28" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B28" s="7">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>12</v>
       </c>
       <c r="C28" s="7">
@@ -9437,51 +9434,51 @@
         <v>2.899053227347741</v>
       </c>
       <c r="E28" s="18">
-        <v>0.26967806466165845</v>
+        <v>0.26967805907043779</v>
       </c>
       <c r="F28" s="7">
-        <f t="shared" si="4"/>
-        <v>0.11313296229230563</v>
+        <f t="shared" si="6"/>
+        <v>0.11313299443948255</v>
       </c>
       <c r="G28" s="7"/>
       <c r="H28" s="7">
         <v>5.2098428893790585</v>
       </c>
       <c r="I28" s="15">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>4.9098428893790587</v>
       </c>
       <c r="J28" s="16">
         <v>1000</v>
       </c>
       <c r="K28" s="15">
-        <f t="shared" si="6"/>
-        <v>12.360417326524809</v>
+        <f t="shared" si="9"/>
+        <v>12.360417250195674</v>
       </c>
       <c r="L28" s="7">
         <f t="shared" si="2"/>
-        <v>0.15277991648585471</v>
+        <v>0.15277991459893481</v>
       </c>
       <c r="M28" s="7">
         <f t="shared" si="3"/>
-        <v>0.3099483205972931</v>
+        <v>0.30994831480241403</v>
       </c>
       <c r="N28" s="15">
-        <f>-I28</f>
+        <f t="shared" si="4"/>
         <v>-4.9098428893790587</v>
       </c>
       <c r="O28" s="13">
-        <f>E28*mass*K28</f>
-        <v>500.00001345414614</v>
+        <f t="shared" si="5"/>
+        <v>500.00000000002905</v>
       </c>
       <c r="P28" s="21">
-        <f>IF(O28&gt;0,P27+O28*(B28-B27),P27)</f>
-        <v>4750.0007200019836</v>
+        <f t="shared" si="7"/>
+        <v>4750.0000000015752</v>
       </c>
     </row>
-    <row r="29" spans="2:19" x14ac:dyDescent="0.45">
+    <row r="29" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B29" s="7">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>12.5</v>
       </c>
       <c r="C29" s="7">
@@ -9492,51 +9489,51 @@
         <v>2.899053227347741</v>
       </c>
       <c r="E29" s="18">
-        <v>0.26844952458160359</v>
+        <v>0.268449520522833</v>
       </c>
       <c r="F29" s="7">
-        <f t="shared" si="4"/>
-        <v>8.3873014330087425E-2</v>
+        <f t="shared" si="6"/>
+        <v>8.3873040199002435E-2</v>
       </c>
       <c r="G29" s="7"/>
       <c r="H29" s="7">
         <v>5.5194264374166675</v>
       </c>
       <c r="I29" s="15">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>5.2194264374166677</v>
       </c>
       <c r="J29" s="16">
         <v>1000</v>
       </c>
       <c r="K29" s="15">
-        <f t="shared" si="6"/>
-        <v>12.416983807670961</v>
+        <f t="shared" si="9"/>
+        <v>12.416983747415415</v>
       </c>
       <c r="L29" s="7">
         <f t="shared" si="2"/>
-        <v>0.15418148687996286</v>
+        <v>0.15418148538357856</v>
       </c>
       <c r="M29" s="7">
         <f t="shared" si="3"/>
-        <v>0.30957564204020505</v>
+        <v>0.30957563777536756</v>
       </c>
       <c r="N29" s="15">
-        <f>-I29</f>
+        <f t="shared" si="4"/>
         <v>-5.2194264374166677</v>
       </c>
       <c r="O29" s="13">
-        <f>E29*mass*K29</f>
-        <v>500.00000998601092</v>
+        <f t="shared" si="5"/>
+        <v>500.00000000002171</v>
       </c>
       <c r="P29" s="21">
-        <f>IF(O29&gt;0,P28+O29*(B29-B28),P28)</f>
-        <v>5000.0007249949895</v>
+        <f t="shared" si="7"/>
+        <v>5000.0000000015862</v>
       </c>
     </row>
-    <row r="30" spans="2:19" x14ac:dyDescent="0.45">
+    <row r="30" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B30" s="7">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>13</v>
       </c>
       <c r="C30" s="7">
@@ -9547,51 +9544,51 @@
         <v>2.899053227347741</v>
       </c>
       <c r="E30" s="18">
-        <v>0.26754592682403278</v>
+        <v>0.26754592386506326</v>
       </c>
       <c r="F30" s="7">
-        <f t="shared" si="4"/>
-        <v>6.2105245943107512E-2</v>
+        <f t="shared" si="6"/>
+        <v>6.2105266566924833E-2</v>
       </c>
       <c r="G30" s="7"/>
       <c r="H30" s="7">
         <v>5.1096925870788503</v>
       </c>
       <c r="I30" s="15">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>4.8096925870788505</v>
       </c>
       <c r="J30" s="16">
         <v>1000</v>
       </c>
       <c r="K30" s="15">
-        <f t="shared" si="6"/>
-        <v>12.458920314836005</v>
+        <f t="shared" si="9"/>
+        <v>12.458920267514916</v>
       </c>
       <c r="L30" s="7">
         <f t="shared" si="2"/>
-        <v>0.15522469541143333</v>
+        <v>0.15522469423229396</v>
       </c>
       <c r="M30" s="7">
         <f t="shared" si="3"/>
-        <v>0.30931461172357011</v>
+        <v>0.30931460857243614</v>
       </c>
       <c r="N30" s="15">
-        <f>-I30</f>
+        <f t="shared" si="4"/>
         <v>-4.8096925870788505</v>
       </c>
       <c r="O30" s="13">
-        <f>E30*mass*K30</f>
-        <v>500.00000742893536</v>
+        <f t="shared" si="5"/>
+        <v>500.00000000001592</v>
       </c>
       <c r="P30" s="21">
-        <f>IF(O30&gt;0,P29+O30*(B30-B29),P29)</f>
-        <v>5250.0007287094568</v>
+        <f t="shared" si="7"/>
+        <v>5250.0000000015943</v>
       </c>
     </row>
-    <row r="31" spans="2:19" x14ac:dyDescent="0.45">
+    <row r="31" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B31" s="7">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>13.5</v>
       </c>
       <c r="C31" s="7">
@@ -9602,51 +9599,51 @@
         <v>2.899053227347741</v>
       </c>
       <c r="E31" s="18">
-        <v>0.2668807520109866</v>
+        <v>0.26688074984697091</v>
       </c>
       <c r="F31" s="7">
-        <f t="shared" si="4"/>
-        <v>4.594549961542338E-2</v>
+        <f t="shared" si="6"/>
+        <v>4.5945515941154813E-2</v>
       </c>
       <c r="G31" s="7"/>
       <c r="H31" s="7">
         <v>5.3191209663056442</v>
       </c>
       <c r="I31" s="15">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>5.0191209663056444</v>
       </c>
       <c r="J31" s="16">
         <v>1000</v>
       </c>
       <c r="K31" s="15">
-        <f t="shared" si="6"/>
-        <v>12.489972937807559</v>
+        <f t="shared" si="9"/>
+        <v>12.489972900798378</v>
       </c>
       <c r="L31" s="7">
         <f t="shared" si="2"/>
-        <v>0.15599942398716518</v>
+        <v>0.15599942306267783</v>
       </c>
       <c r="M31" s="7">
         <f t="shared" si="3"/>
-        <v>0.30912967518223977</v>
+        <v>0.3091296728474473</v>
       </c>
       <c r="N31" s="15">
-        <f>-I31</f>
+        <f t="shared" si="4"/>
         <v>-5.0191209663056444</v>
       </c>
       <c r="O31" s="13">
-        <f>E31*mass*K31</f>
-        <v>500.00000553584294</v>
+        <f t="shared" si="5"/>
+        <v>500.00000000001262</v>
       </c>
       <c r="P31" s="21">
-        <f>IF(O31&gt;0,P30+O31*(B31-B30),P30)</f>
-        <v>5500.0007314773784</v>
+        <f t="shared" si="7"/>
+        <v>5500.0000000016007</v>
       </c>
     </row>
-    <row r="32" spans="2:19" x14ac:dyDescent="0.45">
+    <row r="32" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B32" s="7">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>14</v>
       </c>
       <c r="C32" s="7">
@@ -9657,51 +9654,51 @@
         <v>2.899053227347741</v>
       </c>
       <c r="E32" s="18">
-        <v>0.26639077992376387</v>
+        <v>0.26639077833742736</v>
       </c>
       <c r="F32" s="7">
-        <f t="shared" si="4"/>
-        <v>3.3967811647312107E-2</v>
+        <f t="shared" si="6"/>
+        <v>3.3967824499070876E-2</v>
       </c>
       <c r="G32" s="7"/>
       <c r="H32" s="7">
         <v>5.0302252538942218</v>
       </c>
       <c r="I32" s="15">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>4.730225253894222</v>
       </c>
       <c r="J32" s="16">
         <v>1000</v>
       </c>
       <c r="K32" s="15">
-        <f t="shared" si="6"/>
-        <v>12.512945687615272</v>
+        <f t="shared" si="9"/>
+        <v>12.512945658768956</v>
       </c>
       <c r="L32" s="7">
         <f t="shared" si="2"/>
-        <v>0.15657380978120963</v>
+        <v>0.15657380905930487</v>
       </c>
       <c r="M32" s="7">
         <f t="shared" si="3"/>
-        <v>0.30899741995329605</v>
+        <v>0.3089974182198939</v>
       </c>
       <c r="N32" s="15">
-        <f>-I32</f>
+        <f t="shared" si="4"/>
         <v>-4.730225253894222</v>
       </c>
       <c r="O32" s="13">
-        <f>E32*mass*K32</f>
-        <v>500.00000413012947</v>
+        <f t="shared" si="5"/>
+        <v>500.00000000000927</v>
       </c>
       <c r="P32" s="21">
-        <f>IF(O32&gt;0,P31+O32*(B32-B31),P31)</f>
-        <v>5750.0007335424434</v>
+        <f t="shared" si="7"/>
+        <v>5750.0000000016053</v>
       </c>
     </row>
-    <row r="33" spans="2:18" x14ac:dyDescent="0.45">
+    <row r="33" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B33" s="7">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>14.5</v>
       </c>
       <c r="C33" s="7">
@@ -9712,51 +9709,51 @@
         <v>2.899053227347741</v>
       </c>
       <c r="E33" s="18">
-        <v>0.26602969546127081</v>
+        <v>0.26602969429639273</v>
       </c>
       <c r="F33" s="7">
-        <f t="shared" si="4"/>
-        <v>2.5100210478279816E-2</v>
+        <f t="shared" si="6"/>
+        <v>2.5100220550460683E-2</v>
       </c>
       <c r="G33" s="7"/>
       <c r="H33" s="7">
         <v>5.7922039382197701</v>
       </c>
       <c r="I33" s="15">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>5.4922039382197703</v>
       </c>
       <c r="J33" s="16">
         <v>1000</v>
       </c>
       <c r="K33" s="15">
-        <f t="shared" si="6"/>
-        <v>12.529929593438927</v>
+        <f t="shared" si="9"/>
+        <v>12.529929571018492</v>
       </c>
       <c r="L33" s="7">
         <f t="shared" si="2"/>
-        <v>0.15699913561653658</v>
+        <v>0.15699913505468366</v>
       </c>
       <c r="M33" s="7">
         <f t="shared" si="3"/>
-        <v>0.30890213248139958</v>
+        <v>0.30890213119263354</v>
       </c>
       <c r="N33" s="15">
-        <f>-I33</f>
+        <f t="shared" si="4"/>
         <v>-5.4922039382197703</v>
       </c>
       <c r="O33" s="13">
-        <f>E33*mass*K33</f>
-        <v>500.00000308405839</v>
+        <f t="shared" si="5"/>
+        <v>500.00000000000711</v>
       </c>
       <c r="P33" s="21">
-        <f>IF(O33&gt;0,P32+O33*(B33-B32),P32)</f>
-        <v>6000.0007350844726</v>
+        <f t="shared" si="7"/>
+        <v>6000.0000000016089</v>
       </c>
     </row>
-    <row r="34" spans="2:18" x14ac:dyDescent="0.45">
+    <row r="34" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B34" s="7">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>15</v>
       </c>
       <c r="C34" s="7">
@@ -9767,51 +9764,51 @@
         <v>2.899053227347741</v>
       </c>
       <c r="E34" s="18">
-        <v>0.26576350361143186</v>
+        <v>0.26576350275494681</v>
       </c>
       <c r="F34" s="7">
-        <f t="shared" si="4"/>
-        <v>1.8540791124143752E-2</v>
+        <f t="shared" si="6"/>
+        <v>1.854079898937E-2</v>
       </c>
       <c r="G34" s="7"/>
       <c r="H34" s="7">
         <v>5.51718919013455</v>
       </c>
       <c r="I34" s="15">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>5.2171891901345502</v>
       </c>
       <c r="J34" s="16">
         <v>1000</v>
       </c>
       <c r="K34" s="15">
-        <f t="shared" si="6"/>
-        <v>12.542479698678067</v>
+        <f t="shared" si="9"/>
+        <v>12.542479681293722</v>
       </c>
       <c r="L34" s="7">
         <f t="shared" si="2"/>
-        <v>0.15731379699175144</v>
+        <v>0.15731379655566588</v>
       </c>
       <c r="M34" s="7">
         <f t="shared" si="3"/>
-        <v>0.3088330788237969</v>
+        <v>0.30883307786462261</v>
       </c>
       <c r="N34" s="15">
-        <f>-I34</f>
+        <f t="shared" si="4"/>
         <v>-5.2171891901345502</v>
       </c>
       <c r="O34" s="13">
-        <f>E34*mass*K34</f>
-        <v>500.00000230439082</v>
+        <f t="shared" si="5"/>
+        <v>500.00000000000529</v>
       </c>
       <c r="P34" s="21">
-        <f>IF(O34&gt;0,P33+O34*(B34-B33),P33)</f>
-        <v>6250.0007362366678</v>
+        <f t="shared" si="7"/>
+        <v>6250.0000000016116</v>
       </c>
     </row>
-    <row r="35" spans="2:18" x14ac:dyDescent="0.45">
+    <row r="35" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B35" s="7">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>15.5</v>
       </c>
       <c r="C35" s="7">
@@ -9825,50 +9822,50 @@
         <v>0</v>
       </c>
       <c r="F35" s="7">
-        <f t="shared" si="4"/>
-        <v>-0.25187538121740527</v>
+        <f t="shared" si="6"/>
+        <v>-0.25187537446369479</v>
       </c>
       <c r="G35" s="7"/>
       <c r="H35" s="7">
         <v>5.7184578283483321</v>
       </c>
       <c r="I35" s="15">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>5.4184578283483322</v>
       </c>
       <c r="J35" s="16">
         <v>1000</v>
       </c>
       <c r="K35" s="15">
-        <f t="shared" si="6"/>
-        <v>12.551750094240138</v>
+        <f t="shared" si="9"/>
+        <v>12.551750080788407</v>
       </c>
       <c r="L35" s="7">
         <f t="shared" si="2"/>
-        <v>0.15754643042825731</v>
+        <v>0.15754643009057179</v>
       </c>
       <c r="M35" s="7">
         <f t="shared" si="3"/>
-        <v>0.15754643042825731</v>
+        <v>0.15754643009057179</v>
       </c>
       <c r="N35" s="15">
-        <f>-I35</f>
+        <f t="shared" si="4"/>
         <v>-5.4184578283483322</v>
       </c>
       <c r="O35" s="13">
-        <f>E35*mass*K35</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="P35" s="21">
-        <f>IF(O35&gt;0,P34+O35*(B35-B34),P34)</f>
-        <v>6250.0007362366678</v>
+        <f t="shared" si="7"/>
+        <v>6250.0000000016116</v>
       </c>
     </row>
-    <row r="39" spans="2:18" x14ac:dyDescent="0.45">
+    <row r="39" spans="2:18" x14ac:dyDescent="0.25">
       <c r="Q39" s="7"/>
       <c r="R39" s="7"/>
     </row>
-    <row r="40" spans="2:18" x14ac:dyDescent="0.45">
+    <row r="40" spans="2:18" x14ac:dyDescent="0.25">
       <c r="Q40" s="7"/>
       <c r="R40" s="7"/>
     </row>
@@ -9909,9 +9906,9 @@
       <selection activeCell="D84" sqref="D84"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:13" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>18</v>
       </c>
@@ -9920,7 +9917,7 @@
         <v>68.556546004010443</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>15</v>
       </c>
@@ -9935,16 +9932,16 @@
         <v>68.556546004010443</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="6">
         <v>0</v>
       </c>
       <c r="B3" s="7">
-        <f>6*COS(A3)</f>
+        <f t="shared" ref="B3:B34" si="0">6*COS(A3)</f>
         <v>6</v>
       </c>
       <c r="C3" s="8">
-        <f>6*SIN(A3)</f>
+        <f t="shared" ref="C3:C34" si="1">6*SIN(A3)</f>
         <v>0</v>
       </c>
       <c r="M3">
@@ -9952,17 +9949,17 @@
         <v>68.556546004010443</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" s="6">
         <f>2*3.14/31</f>
         <v>0.20258064516129032</v>
       </c>
       <c r="B4" s="7">
-        <f>6*COS(A4)</f>
+        <f t="shared" si="0"/>
         <v>5.877303719254698</v>
       </c>
       <c r="C4" s="8">
-        <f>6*SIN(A4)</f>
+        <f t="shared" si="1"/>
         <v>1.2071872231078726</v>
       </c>
       <c r="D4" s="7"/>
@@ -9971,17 +9968,17 @@
         <v>68.556546004010443</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="6">
-        <f>0.2025+A4</f>
+        <f t="shared" ref="A5:A34" si="2">0.2025+A4</f>
         <v>0.40508064516129033</v>
       </c>
       <c r="B5" s="7">
-        <f>6*COS(A5)</f>
+        <f t="shared" si="0"/>
         <v>5.5144237108234266</v>
       </c>
       <c r="C5" s="8">
-        <f>6*SIN(A5)</f>
+        <f t="shared" si="1"/>
         <v>2.3645572815029006</v>
       </c>
       <c r="D5" s="7"/>
@@ -9990,17 +9987,17 @@
         <v>68.556546004010443</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="6">
-        <f>0.2025+A5</f>
+        <f t="shared" si="2"/>
         <v>0.6075806451612904</v>
       </c>
       <c r="B6" s="7">
-        <f>6*COS(A6)</f>
+        <f t="shared" si="0"/>
         <v>4.9261895240539069</v>
       </c>
       <c r="C6" s="8">
-        <f>6*SIN(A6)</f>
+        <f t="shared" si="1"/>
         <v>3.4252965963696544</v>
       </c>
       <c r="D6" s="7"/>
@@ -10009,17 +10006,17 @@
         <v>68.556546004010443</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" s="6">
-        <f>0.2025+A6</f>
+        <f t="shared" si="2"/>
         <v>0.81008064516129041</v>
       </c>
       <c r="B7" s="7">
-        <f>6*COS(A7)</f>
+        <f t="shared" si="0"/>
         <v>4.136640122722123</v>
       </c>
       <c r="C7" s="8">
-        <f>6*SIN(A7)</f>
+        <f t="shared" si="1"/>
         <v>4.3460566603629891</v>
       </c>
       <c r="D7" s="7"/>
@@ -10028,17 +10025,17 @@
         <v>68.556546004010443</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" s="6">
-        <f>0.2025+A7</f>
+        <f t="shared" si="2"/>
         <v>1.0125806451612904</v>
       </c>
       <c r="B8" s="7">
-        <f>6*COS(A8)</f>
+        <f t="shared" si="0"/>
         <v>3.1780414816470484</v>
       </c>
       <c r="C8" s="8">
-        <f>6*SIN(A8)</f>
+        <f t="shared" si="1"/>
         <v>5.0892094023463637</v>
       </c>
       <c r="D8" s="7"/>
@@ -10047,17 +10044,17 @@
         <v>68.556546004010443</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" s="6">
-        <f>0.2025+A8</f>
+        <f t="shared" si="2"/>
         <v>1.2150806451612906</v>
       </c>
       <c r="B9" s="7">
-        <f>6*COS(A9)</f>
+        <f t="shared" si="0"/>
         <v>2.0895679951886281</v>
       </c>
       <c r="C9" s="8">
-        <f>6*SIN(A9)</f>
+        <f t="shared" si="1"/>
         <v>5.6243849080129085</v>
       </c>
       <c r="D9" s="7"/>
@@ -10066,17 +10063,17 @@
         <v>68.556546004010443</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" s="6">
-        <f>0.2025+A9</f>
+        <f t="shared" si="2"/>
         <v>1.4175806451612907</v>
       </c>
       <c r="B10" s="7">
-        <f>6*COS(A10)</f>
+        <f t="shared" si="0"/>
         <v>0.91570156409423631</v>
       </c>
       <c r="C10" s="8">
-        <f>6*SIN(A10)</f>
+        <f t="shared" si="1"/>
         <v>5.929712526380631</v>
       </c>
       <c r="D10" s="7"/>
@@ -10085,17 +10082,17 @@
         <v>4.8476798574163293</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" s="6">
-        <f>0.2025+A10</f>
+        <f t="shared" si="2"/>
         <v>1.6200806451612908</v>
       </c>
       <c r="B11" s="7">
-        <f>6*COS(A11)</f>
+        <f t="shared" si="0"/>
         <v>-0.29558621588462353</v>
       </c>
       <c r="C11" s="8">
-        <f>6*SIN(A11)</f>
+        <f t="shared" si="1"/>
         <v>5.9927146427123503</v>
       </c>
       <c r="D11" s="7"/>
@@ -10104,17 +10101,17 @@
         <v>4.8476798574163293</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" s="6">
-        <f>0.2025+A11</f>
+        <f t="shared" si="2"/>
         <v>1.8225806451612909</v>
       </c>
       <c r="B12" s="7">
-        <f>6*COS(A12)</f>
+        <f t="shared" si="0"/>
         <v>-1.4947944763521246</v>
       </c>
       <c r="C12" s="8">
-        <f>6*SIN(A12)</f>
+        <f t="shared" si="1"/>
         <v>5.8108165926543558</v>
       </c>
       <c r="D12" s="7"/>
@@ -10123,17 +10120,17 @@
         <v>4.8476798574163293</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" s="6">
-        <f>0.2025+A12</f>
+        <f t="shared" si="2"/>
         <v>2.025080645161291</v>
       </c>
       <c r="B13" s="7">
-        <f>6*COS(A13)</f>
+        <f t="shared" si="0"/>
         <v>-2.6329159943660638</v>
       </c>
       <c r="C13" s="8">
-        <f>6*SIN(A13)</f>
+        <f t="shared" si="1"/>
         <v>5.39145187928181</v>
       </c>
       <c r="D13" s="7"/>
@@ -10142,17 +10139,17 @@
         <v>68.556546004010443</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" s="6">
-        <f>0.2025+A13</f>
+        <f t="shared" si="2"/>
         <v>2.2275806451612912</v>
       </c>
       <c r="B14" s="7">
-        <f>6*COS(A14)</f>
+        <f t="shared" si="0"/>
         <v>-3.6634399370650295</v>
       </c>
       <c r="C14" s="8">
-        <f>6*SIN(A14)</f>
+        <f t="shared" si="1"/>
         <v>4.7517583932179228</v>
       </c>
       <c r="D14" s="7"/>
@@ -10161,17 +10158,17 @@
         <v>68.556546004010443</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" s="6">
-        <f>0.2025+A14</f>
+        <f t="shared" si="2"/>
         <v>2.4300806451612913</v>
       </c>
       <c r="B15" s="7">
-        <f>6*COS(A15)</f>
+        <f t="shared" si="0"/>
         <v>-4.5442525880312932</v>
       </c>
       <c r="C15" s="8">
-        <f>6*SIN(A15)</f>
+        <f t="shared" si="1"/>
         <v>3.9178780501913151</v>
       </c>
       <c r="D15" s="7"/>
@@ -10180,17 +10177,17 @@
         <v>68.556546004010443</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" s="6">
-        <f>0.2025+A15</f>
+        <f t="shared" si="2"/>
         <v>2.6325806451612914</v>
       </c>
       <c r="B16" s="7">
-        <f>6*COS(A16)</f>
+        <f t="shared" si="0"/>
         <v>-5.2393583797064815</v>
       </c>
       <c r="C16" s="8">
-        <f>6*SIN(A16)</f>
+        <f t="shared" si="1"/>
         <v>2.9238884672640086</v>
       </c>
       <c r="D16" s="7"/>
@@ -10199,17 +10196,17 @@
         <v>68.556546004010443</v>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17" s="6">
-        <f>0.2025+A16</f>
+        <f t="shared" si="2"/>
         <v>2.8350806451612915</v>
       </c>
       <c r="B17" s="7">
-        <f>6*COS(A17)</f>
+        <f t="shared" si="0"/>
         <v>-5.7203508996066095</v>
       </c>
       <c r="C17" s="8">
-        <f>6*SIN(A17)</f>
+        <f t="shared" si="1"/>
         <v>1.8104103361862067</v>
       </c>
       <c r="D17" s="7"/>
@@ -10218,17 +10215,17 @@
         <v>68.556546004010443</v>
       </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18" s="6">
-        <f>0.2025+A17</f>
+        <f t="shared" si="2"/>
         <v>3.0375806451612917</v>
       </c>
       <c r="B18" s="7">
-        <f>6*COS(A18)</f>
+        <f t="shared" si="0"/>
         <v>-5.9675737557326025</v>
       </c>
       <c r="C18" s="8">
-        <f>6*SIN(A18)</f>
+        <f t="shared" si="1"/>
         <v>0.62294740539750326</v>
       </c>
       <c r="D18" s="7"/>
@@ -10237,17 +10234,17 @@
         <v>68.556546004010443</v>
       </c>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19" s="6">
-        <f>0.2025+A18</f>
+        <f t="shared" si="2"/>
         <v>3.2400806451612918</v>
       </c>
       <c r="B19" s="7">
-        <f>6*COS(A19)</f>
+        <f t="shared" si="0"/>
         <v>-5.9709238608843673</v>
       </c>
       <c r="C19" s="8">
-        <f>6*SIN(A19)</f>
+        <f t="shared" si="1"/>
         <v>-0.58997309050643787</v>
       </c>
       <c r="D19" s="7"/>
@@ -10256,17 +10253,17 @@
         <v>68.556546004010443</v>
       </c>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20" s="6">
-        <f>0.2025+A19</f>
+        <f t="shared" si="2"/>
         <v>3.4425806451612919</v>
       </c>
       <c r="B20" s="7">
-        <f>6*COS(A20)</f>
+        <f t="shared" si="0"/>
         <v>-5.7302643086083185</v>
       </c>
       <c r="C20" s="8">
-        <f>6*SIN(A20)</f>
+        <f t="shared" si="1"/>
         <v>-1.7787835600459188</v>
       </c>
       <c r="D20" s="7"/>
@@ -10275,17 +10272,17 @@
         <v>68.556546004010443</v>
       </c>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A21" s="6">
-        <f>0.2025+A20</f>
+        <f t="shared" si="2"/>
         <v>3.645080645161292</v>
       </c>
       <c r="B21" s="7">
-        <f>6*COS(A21)</f>
+        <f t="shared" si="0"/>
         <v>-5.255429968059679</v>
       </c>
       <c r="C21" s="8">
-        <f>6*SIN(A21)</f>
+        <f t="shared" si="1"/>
         <v>-2.8949016996817418</v>
       </c>
       <c r="D21" s="7"/>
@@ -10294,17 +10291,17 @@
         <v>68.556546004010443</v>
       </c>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A22" s="6">
-        <f>0.2025+A21</f>
+        <f t="shared" si="2"/>
         <v>3.8475806451612922</v>
       </c>
       <c r="B22" s="7">
-        <f>6*COS(A22)</f>
+        <f t="shared" si="0"/>
         <v>-4.5658255691381679</v>
       </c>
       <c r="C22" s="8">
-        <f>6*SIN(A22)</f>
+        <f t="shared" si="1"/>
         <v>-3.8927158735520528</v>
       </c>
       <c r="D22" s="7"/>
@@ -10313,17 +10310,17 @@
         <v>68.556546004010443</v>
       </c>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A23" s="6">
-        <f>0.2025+A22</f>
+        <f t="shared" si="2"/>
         <v>4.0500806451612918</v>
       </c>
       <c r="B23" s="7">
-        <f>6*COS(A23)</f>
+        <f t="shared" si="0"/>
         <v>-3.6896327026766382</v>
       </c>
       <c r="C23" s="8">
-        <f>6*SIN(A23)</f>
+        <f t="shared" si="1"/>
         <v>-4.7314490929670887</v>
       </c>
       <c r="D23" s="7"/>
@@ -10332,17 +10329,17 @@
         <v>68.556546004010443</v>
       </c>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A24" s="6">
-        <f>0.2025+A23</f>
+        <f t="shared" si="2"/>
         <v>4.2525806451612915</v>
       </c>
       <c r="B24" s="7">
-        <f>6*COS(A24)</f>
+        <f t="shared" si="0"/>
         <v>-2.6626581426630418</v>
       </c>
       <c r="C24" s="8">
-        <f>6*SIN(A24)</f>
+        <f t="shared" si="1"/>
         <v>-5.3768254216879869</v>
       </c>
       <c r="D24" s="7"/>
@@ -10351,17 +10348,17 @@
         <v>68.556546004010443</v>
       </c>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A25" s="6">
-        <f>0.2025+A24</f>
+        <f t="shared" si="2"/>
         <v>4.4550806451612912</v>
       </c>
       <c r="B25" s="7">
-        <f>6*COS(A25)</f>
+        <f t="shared" si="0"/>
         <v>-1.5268705553229922</v>
       </c>
       <c r="C25" s="8">
-        <f>6*SIN(A25)</f>
+        <f t="shared" si="1"/>
         <v>-5.8024707071460222</v>
       </c>
       <c r="D25" s="7"/>
@@ -10370,17 +10367,17 @@
         <v>68.556546004010443</v>
       </c>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A26" s="6">
-        <f>0.2025+A25</f>
+        <f t="shared" si="2"/>
         <v>4.6575806451612909</v>
       </c>
       <c r="B26" s="7">
-        <f>6*COS(A26)</f>
+        <f t="shared" si="0"/>
         <v>-0.32868539437097588</v>
       </c>
       <c r="C26" s="8">
-        <f>6*SIN(A26)</f>
+        <f t="shared" si="1"/>
         <v>-5.9909903948785628</v>
       </c>
       <c r="D26" s="7"/>
@@ -10389,17 +10386,17 @@
         <v>68.556546004010443</v>
       </c>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A27" s="6">
-        <f>0.2025+A26</f>
+        <f t="shared" si="2"/>
         <v>4.8600806451612906</v>
       </c>
       <c r="B27" s="7">
-        <f>6*COS(A27)</f>
+        <f t="shared" si="0"/>
         <v>0.88293192755823768</v>
       </c>
       <c r="C27" s="8">
-        <f>6*SIN(A27)</f>
+        <f t="shared" si="1"/>
         <v>-5.9346803798771077</v>
       </c>
       <c r="D27" s="7"/>
@@ -10408,17 +10405,17 @@
         <v>68.556546004010443</v>
       </c>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A28" s="6">
-        <f>0.2025+A27</f>
+        <f t="shared" si="2"/>
         <v>5.0625806451612902</v>
       </c>
       <c r="B28" s="7">
-        <f>6*COS(A28)</f>
+        <f t="shared" si="0"/>
         <v>2.0584670749035583</v>
       </c>
       <c r="C28" s="8">
-        <f>6*SIN(A28)</f>
+        <f t="shared" si="1"/>
         <v>-5.6358418449720524</v>
       </c>
       <c r="D28" s="7"/>
@@ -10427,17 +10424,17 @@
         <v>68.556546004010443</v>
       </c>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A29" s="6">
-        <f>0.2025+A28</f>
+        <f t="shared" si="2"/>
         <v>5.2650806451612899</v>
       </c>
       <c r="B29" s="7">
-        <f>6*COS(A29)</f>
+        <f t="shared" si="0"/>
         <v>3.1498802576289417</v>
       </c>
       <c r="C29" s="8">
-        <f>6*SIN(A29)</f>
+        <f t="shared" si="1"/>
         <v>-5.1066872199694622</v>
       </c>
       <c r="D29" s="7"/>
@@ -10446,17 +10443,17 @@
         <v>68.556546004010443</v>
       </c>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A30" s="6">
-        <f>0.2025+A29</f>
+        <f t="shared" si="2"/>
         <v>5.4675806451612896</v>
       </c>
       <c r="B30" s="7">
-        <f>6*COS(A30)</f>
+        <f t="shared" si="0"/>
         <v>4.1125694404323383</v>
       </c>
       <c r="C30" s="8">
-        <f>6*SIN(A30)</f>
+        <f t="shared" si="1"/>
         <v>-4.3688411046434323</v>
       </c>
       <c r="D30" s="7"/>
@@ -10465,17 +10462,17 @@
         <v>68.556546004010443</v>
       </c>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A31" s="6">
-        <f>0.2025+A30</f>
+        <f t="shared" si="2"/>
         <v>5.6700806451612893</v>
       </c>
       <c r="B31" s="7">
-        <f>6*COS(A31)</f>
+        <f t="shared" si="0"/>
         <v>4.9071930635855807</v>
       </c>
       <c r="C31" s="8">
-        <f>6*SIN(A31)</f>
+        <f t="shared" si="1"/>
         <v>-3.4524565510224114</v>
       </c>
       <c r="D31" s="7"/>
@@ -10484,17 +10481,17 @@
         <v>68.556546004010443</v>
       </c>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A32" s="6">
-        <f>0.2025+A31</f>
+        <f t="shared" si="2"/>
         <v>5.872580645161289</v>
       </c>
       <c r="B32" s="7">
-        <f>6*COS(A32)</f>
+        <f t="shared" si="0"/>
         <v>5.5012777875205856</v>
       </c>
       <c r="C32" s="8">
-        <f>6*SIN(A32)</f>
+        <f t="shared" si="1"/>
         <v>-2.3949828192562497</v>
       </c>
       <c r="D32" s="7"/>
@@ -10503,32 +10500,32 @@
         <v>68.556546004010443</v>
       </c>
     </row>
-    <row r="33" spans="1:13" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="33" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="6">
-        <f>0.2025+A32</f>
+        <f t="shared" si="2"/>
         <v>6.0750806451612887</v>
       </c>
       <c r="B33" s="7">
-        <f>6*COS(A33)</f>
+        <f t="shared" si="0"/>
         <v>5.8705455585645989</v>
       </c>
       <c r="C33" s="8">
-        <f>6*SIN(A33)</f>
+        <f t="shared" si="1"/>
         <v>-1.2396349643413023</v>
       </c>
       <c r="D33" s="7"/>
     </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A34" s="6">
-        <f>0.2025+A33</f>
+        <f t="shared" si="2"/>
         <v>6.2775806451612883</v>
       </c>
       <c r="B34" s="7">
-        <f>6*COS(A34)</f>
+        <f t="shared" si="0"/>
         <v>5.9999057635376634</v>
       </c>
       <c r="C34" s="8">
-        <f>6*SIN(A34)</f>
+        <f t="shared" si="1"/>
         <v>-3.362779605509747E-2</v>
       </c>
       <c r="D34" s="7"/>
@@ -10536,7 +10533,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="35" spans="1:13" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="35" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" s="9"/>
       <c r="B35" s="10"/>
       <c r="C35" s="11"/>
@@ -10546,187 +10543,187 @@
         <v>0.89905322734774096</v>
       </c>
     </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
       <c r="M36" s="8">
         <f>-Sheet1!E5</f>
         <v>-3.3333333333333335</v>
       </c>
     </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
       <c r="M37" s="8">
         <f>-Sheet1!E6</f>
         <v>-0.81178188793316886</v>
       </c>
     </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
       <c r="M38" s="8">
         <f>-Sheet1!E7</f>
-        <v>-0.57540684173199907</v>
+        <v>-0.57540684173199919</v>
       </c>
     </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:13" x14ac:dyDescent="0.25">
       <c r="M39" s="8">
         <f>-Sheet1!E8</f>
-        <v>-0.46330762212964111</v>
+        <v>-0.46330762212964116</v>
       </c>
     </row>
-    <row r="40" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:13" x14ac:dyDescent="0.25">
       <c r="M40" s="8">
         <f>-Sheet1!E9</f>
         <v>-0.39881017670979807</v>
       </c>
     </row>
-    <row r="41" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:13" x14ac:dyDescent="0.25">
       <c r="M41" s="8">
         <f>-Sheet1!E10</f>
-        <v>2.8506498523458927</v>
+        <v>2.8506498523888202</v>
       </c>
     </row>
-    <row r="42" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:13" x14ac:dyDescent="0.25">
       <c r="M42" s="8">
         <f>-Sheet1!E11</f>
-        <v>5.5973725128120062</v>
+        <v>5.5973725128120009</v>
       </c>
     </row>
-    <row r="43" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="43" spans="1:13" x14ac:dyDescent="0.25">
       <c r="M43" s="8">
         <f>-Sheet1!E12</f>
-        <v>5.0382954994443567</v>
+        <v>5.0382954994443523</v>
       </c>
     </row>
-    <row r="44" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="44" spans="1:13" x14ac:dyDescent="0.25">
       <c r="M44" s="8">
         <f>-Sheet1!E13</f>
-        <v>2.720971899993581</v>
+        <v>2.7209718999853165</v>
       </c>
     </row>
-    <row r="45" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="45" spans="1:13" x14ac:dyDescent="0.25">
       <c r="M45" s="8">
         <f>-Sheet1!E14</f>
-        <v>2.294140882637894</v>
+        <v>2.2941408826284087</v>
       </c>
     </row>
-    <row r="46" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="46" spans="1:13" x14ac:dyDescent="0.25">
       <c r="M46" s="8">
         <f>-Sheet1!E15</f>
-        <v>-0.68827144075126734</v>
+        <v>-0.68827144075275781</v>
       </c>
     </row>
-    <row r="47" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="47" spans="1:13" x14ac:dyDescent="0.25">
       <c r="M47" s="8">
         <f>-Sheet1!E16</f>
-        <v>-0.52065749453026178</v>
+        <v>-0.52065749453103116</v>
       </c>
     </row>
-    <row r="48" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="48" spans="1:13" x14ac:dyDescent="0.25">
       <c r="M48" s="8">
         <f>-Sheet1!E17</f>
-        <v>-0.43278014883945631</v>
+        <v>-0.43278014883994498</v>
       </c>
     </row>
-    <row r="49" spans="13:13" x14ac:dyDescent="0.45">
+    <row r="49" spans="13:13" x14ac:dyDescent="0.25">
       <c r="M49" s="8">
         <f>-Sheet1!E18</f>
-        <v>-0.37987491510003324</v>
+        <v>-0.37987452904105873</v>
       </c>
     </row>
-    <row r="50" spans="13:13" x14ac:dyDescent="0.45">
+    <row r="50" spans="13:13" x14ac:dyDescent="0.25">
       <c r="M50" s="8">
         <f>-Sheet1!E19</f>
-        <v>-0.3456269606042266</v>
+        <v>-0.3456267544683212</v>
       </c>
     </row>
-    <row r="51" spans="13:13" x14ac:dyDescent="0.45">
+    <row r="51" spans="13:13" x14ac:dyDescent="0.25">
       <c r="M51" s="8">
         <f>-Sheet1!E20</f>
-        <v>-0.32248109840558953</v>
+        <v>-0.32248097873156589</v>
       </c>
     </row>
-    <row r="52" spans="13:13" x14ac:dyDescent="0.45">
+    <row r="52" spans="13:13" x14ac:dyDescent="0.25">
       <c r="M52" s="8">
         <f>-Sheet1!E21</f>
-        <v>-0.30640483555087467</v>
+        <v>-0.30640476169421088</v>
       </c>
     </row>
-    <row r="53" spans="13:13" x14ac:dyDescent="0.45">
+    <row r="53" spans="13:13" x14ac:dyDescent="0.25">
       <c r="M53" s="8">
         <f>-Sheet1!E22</f>
-        <v>-0.2950351658610682</v>
+        <v>-0.29503511815930472</v>
       </c>
     </row>
-    <row r="54" spans="13:13" x14ac:dyDescent="0.45">
+    <row r="54" spans="13:13" x14ac:dyDescent="0.25">
       <c r="M54" s="8">
         <f>-Sheet1!E23</f>
-        <v>-0.2868947046668639</v>
+        <v>-0.2868946727906857</v>
       </c>
     </row>
-    <row r="55" spans="13:13" x14ac:dyDescent="0.45">
+    <row r="55" spans="13:13" x14ac:dyDescent="0.25">
       <c r="M55" s="8">
         <f>-Sheet1!E24</f>
-        <v>-0.28101637663437412</v>
+        <v>-0.28101635478366221</v>
       </c>
     </row>
-    <row r="56" spans="13:13" x14ac:dyDescent="0.45">
+    <row r="56" spans="13:13" x14ac:dyDescent="0.25">
       <c r="M56" s="8">
         <f>-Sheet1!E25</f>
-        <v>-0.27674599253790766</v>
+        <v>-0.2767459772718156</v>
       </c>
     </row>
-    <row r="57" spans="13:13" x14ac:dyDescent="0.45">
+    <row r="57" spans="13:13" x14ac:dyDescent="0.25">
       <c r="M57" s="8">
         <f>-Sheet1!E26</f>
-        <v>-0.27363041899152879</v>
+        <v>-0.27363040817363604</v>
       </c>
     </row>
-    <row r="58" spans="13:13" x14ac:dyDescent="0.45">
+    <row r="58" spans="13:13" x14ac:dyDescent="0.25">
       <c r="M58" s="8">
         <f>-Sheet1!E27</f>
-        <v>-0.27135037058589395</v>
+        <v>-0.27135036283896757</v>
       </c>
     </row>
-    <row r="59" spans="13:13" x14ac:dyDescent="0.45">
+    <row r="59" spans="13:13" x14ac:dyDescent="0.25">
       <c r="M59" s="8">
         <f>-Sheet1!E28</f>
-        <v>-0.26967806466165845</v>
+        <v>-0.26967805907043779</v>
       </c>
     </row>
-    <row r="60" spans="13:13" x14ac:dyDescent="0.45">
+    <row r="60" spans="13:13" x14ac:dyDescent="0.25">
       <c r="M60" s="8">
         <f>-Sheet1!E29</f>
-        <v>-0.26844952458160359</v>
+        <v>-0.268449520522833</v>
       </c>
     </row>
-    <row r="61" spans="13:13" x14ac:dyDescent="0.45">
+    <row r="61" spans="13:13" x14ac:dyDescent="0.25">
       <c r="M61" s="8">
         <f>-Sheet1!E30</f>
-        <v>-0.26754592682403278</v>
+        <v>-0.26754592386506326</v>
       </c>
     </row>
-    <row r="62" spans="13:13" x14ac:dyDescent="0.45">
+    <row r="62" spans="13:13" x14ac:dyDescent="0.25">
       <c r="M62" s="8">
         <f>-Sheet1!E31</f>
-        <v>-0.2668807520109866</v>
+        <v>-0.26688074984697091</v>
       </c>
     </row>
-    <row r="63" spans="13:13" x14ac:dyDescent="0.45">
+    <row r="63" spans="13:13" x14ac:dyDescent="0.25">
       <c r="M63" s="8">
         <f>-Sheet1!E32</f>
-        <v>-0.26639077992376387</v>
+        <v>-0.26639077833742736</v>
       </c>
     </row>
-    <row r="64" spans="13:13" x14ac:dyDescent="0.45">
+    <row r="64" spans="13:13" x14ac:dyDescent="0.25">
       <c r="M64" s="8">
         <f>-Sheet1!E33</f>
-        <v>-0.26602969546127081</v>
+        <v>-0.26602969429639273</v>
       </c>
     </row>
-    <row r="65" spans="13:13" x14ac:dyDescent="0.45">
+    <row r="65" spans="13:13" x14ac:dyDescent="0.25">
       <c r="M65" s="8">
         <f>-Sheet1!E34</f>
-        <v>-0.26576350361143186</v>
+        <v>-0.26576350275494681</v>
       </c>
     </row>
-    <row r="66" spans="13:13" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="66" spans="13:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="M66" s="11">
         <f>-Sheet1!E35</f>
         <v>0</v>

</xml_diff>